<commit_message>
updated most charts and added RRm
</commit_message>
<xml_diff>
--- a/out.xlsx
+++ b/out.xlsx
@@ -8,16 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\uphjan2\Projects\screen-audit\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5CE914D9-ADFE-4591-B0EC-4D20CBBF4525}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F143F62-DBF6-473E-9F31-05DF42421C89}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-24120" yWindow="-120" windowWidth="24240" windowHeight="13140" tabRatio="500" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-24120" yWindow="-120" windowWidth="24240" windowHeight="13140" tabRatio="500" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="out" sheetId="1" r:id="rId1"/>
     <sheet name="utwist" sheetId="2" r:id="rId2"/>
     <sheet name="RRm" sheetId="3" r:id="rId3"/>
-    <sheet name="FAR-csf" sheetId="4" r:id="rId4"/>
-    <sheet name="FAR-con" sheetId="5" r:id="rId5"/>
+    <sheet name="FAR-rrm" sheetId="6" r:id="rId4"/>
+    <sheet name="FAR-csf" sheetId="4" r:id="rId5"/>
+    <sheet name="FAR-con" sheetId="5" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="245" uniqueCount="87">
   <si>
     <t>trial</t>
   </si>
@@ -289,6 +290,15 @@
   </si>
   <si>
     <t>Screen</t>
+  </si>
+  <si>
+    <t>RRv</t>
+  </si>
+  <si>
+    <t>feedcst</t>
+  </si>
+  <si>
+    <t>SD</t>
   </si>
 </sst>
 </file>
@@ -844,7 +854,7 @@
   <dimension ref="A1:AMJ22"/>
   <sheetViews>
     <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="G26" sqref="G26"/>
+      <selection activeCell="R22" sqref="R22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2709,7 +2719,7 @@
   <dimension ref="A1:S20"/>
   <sheetViews>
     <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection sqref="A1:A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3170,11 +3180,219 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2F084A57-A247-4047-A2D6-323408F344BB}">
+  <dimension ref="A1:H10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D1" sqref="D1:E10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="3" max="3" width="9.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="8.88671875" style="8"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1" s="21" t="s">
+        <v>66</v>
+      </c>
+      <c r="B1" s="21" t="s">
+        <v>83</v>
+      </c>
+      <c r="C1" s="21" t="s">
+        <v>85</v>
+      </c>
+      <c r="D1" s="21" t="s">
+        <v>84</v>
+      </c>
+      <c r="E1" s="21" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A2" s="8">
+        <v>1</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>80</v>
+      </c>
+      <c r="C2" s="8">
+        <v>1.38</v>
+      </c>
+      <c r="D2" s="4">
+        <v>25.081389940867716</v>
+      </c>
+      <c r="E2" s="4">
+        <v>41.438818163172755</v>
+      </c>
+      <c r="G2" s="4"/>
+      <c r="H2" s="4"/>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3" s="8">
+        <v>2</v>
+      </c>
+      <c r="B3" s="8" t="s">
+        <v>80</v>
+      </c>
+      <c r="C3" s="8">
+        <v>1.62</v>
+      </c>
+      <c r="D3" s="4">
+        <v>25.025977140116694</v>
+      </c>
+      <c r="E3" s="4">
+        <v>40.319629836854681</v>
+      </c>
+      <c r="G3" s="4"/>
+      <c r="H3" s="4"/>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A4" s="8">
+        <v>3</v>
+      </c>
+      <c r="B4" s="8" t="s">
+        <v>80</v>
+      </c>
+      <c r="C4" s="8">
+        <v>0.98</v>
+      </c>
+      <c r="D4" s="4">
+        <v>25.122205745043114</v>
+      </c>
+      <c r="E4" s="4">
+        <v>35.632516311846864</v>
+      </c>
+      <c r="G4" s="4"/>
+      <c r="H4" s="4"/>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A5" s="8">
+        <v>1</v>
+      </c>
+      <c r="B5" s="8" t="s">
+        <v>81</v>
+      </c>
+      <c r="C5" s="8">
+        <v>1.08</v>
+      </c>
+      <c r="D5" s="4">
+        <v>22.027475130270012</v>
+      </c>
+      <c r="E5" s="4">
+        <v>43.686509816306121</v>
+      </c>
+      <c r="G5" s="4"/>
+      <c r="H5" s="4"/>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A6" s="8">
+        <v>2</v>
+      </c>
+      <c r="B6" s="8" t="s">
+        <v>81</v>
+      </c>
+      <c r="C6" s="8">
+        <v>1.34</v>
+      </c>
+      <c r="D6" s="4">
+        <v>22.0036790717419</v>
+      </c>
+      <c r="E6" s="4">
+        <v>47.032349220362029</v>
+      </c>
+      <c r="G6" s="4"/>
+      <c r="H6" s="4"/>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A7" s="8">
+        <v>3</v>
+      </c>
+      <c r="B7" s="8" t="s">
+        <v>81</v>
+      </c>
+      <c r="C7" s="8">
+        <v>0.8</v>
+      </c>
+      <c r="D7" s="4">
+        <v>21.969909354265958</v>
+      </c>
+      <c r="E7" s="4">
+        <v>41.47743201569947</v>
+      </c>
+      <c r="G7" s="4"/>
+      <c r="H7" s="4"/>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A8" s="8">
+        <v>1</v>
+      </c>
+      <c r="B8" s="8" t="s">
+        <v>82</v>
+      </c>
+      <c r="C8" s="8">
+        <v>0.91</v>
+      </c>
+      <c r="D8" s="4">
+        <v>42.03389830508474</v>
+      </c>
+      <c r="E8" s="4">
+        <v>70.210467498603094</v>
+      </c>
+      <c r="G8" s="4"/>
+      <c r="H8" s="4"/>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A9" s="8">
+        <v>2</v>
+      </c>
+      <c r="B9" s="8" t="s">
+        <v>82</v>
+      </c>
+      <c r="C9" s="8">
+        <v>1.1200000000000001</v>
+      </c>
+      <c r="D9" s="4">
+        <v>41.83347838700319</v>
+      </c>
+      <c r="E9" s="4">
+        <v>72.088047577603703</v>
+      </c>
+      <c r="G9" s="4"/>
+      <c r="H9" s="4"/>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A10" s="8">
+        <v>3</v>
+      </c>
+      <c r="B10" s="8" t="s">
+        <v>82</v>
+      </c>
+      <c r="C10" s="8">
+        <v>0.64</v>
+      </c>
+      <c r="D10" s="4">
+        <v>38.324386503067487</v>
+      </c>
+      <c r="E10" s="4">
+        <v>58.684216832822088</v>
+      </c>
+      <c r="G10" s="4"/>
+      <c r="H10" s="4"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{44A527B7-36FC-4EDF-99B8-F5F2E7B3CFF4}">
-  <dimension ref="A1:E10"/>
+  <dimension ref="A1:G18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H27" sqref="H27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3182,7 +3400,7 @@
     <col min="1" max="16384" width="8.88671875" style="8"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="21" t="s">
         <v>66</v>
       </c>
@@ -3198,8 +3416,14 @@
       <c r="E1" s="21" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F1" s="21" t="s">
+        <v>84</v>
+      </c>
+      <c r="G1" s="21" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="8">
         <v>1</v>
       </c>
@@ -3218,8 +3442,14 @@
         <f>out!F3</f>
         <v>360</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F2" s="4">
+        <v>25.081389940867716</v>
+      </c>
+      <c r="G2" s="4">
+        <v>41.438818163172755</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" s="8">
         <v>2</v>
       </c>
@@ -3238,8 +3468,14 @@
         <f>out!F10</f>
         <v>393</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F3" s="4">
+        <v>25.025977140116694</v>
+      </c>
+      <c r="G3" s="4">
+        <v>40.319629836854681</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" s="8">
         <v>3</v>
       </c>
@@ -3258,8 +3494,14 @@
         <f>out!F17</f>
         <v>345</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F4" s="4">
+        <v>25.122205745043114</v>
+      </c>
+      <c r="G4" s="4">
+        <v>35.632516311846864</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" s="8">
         <v>1</v>
       </c>
@@ -3278,8 +3520,14 @@
         <f>out!F6</f>
         <v>138</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F5" s="4">
+        <v>22.027475130270012</v>
+      </c>
+      <c r="G5" s="4">
+        <v>43.686509816306121</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" s="8">
         <v>2</v>
       </c>
@@ -3298,8 +3546,14 @@
         <f>out!F13</f>
         <v>214</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F6" s="4">
+        <v>22.0036790717419</v>
+      </c>
+      <c r="G6" s="4">
+        <v>47.032349220362029</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" s="8">
         <v>3</v>
       </c>
@@ -3318,8 +3572,14 @@
         <f>out!F20</f>
         <v>176</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F7" s="4">
+        <v>21.969909354265958</v>
+      </c>
+      <c r="G7" s="4">
+        <v>41.47743201569947</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" s="8">
         <v>1</v>
       </c>
@@ -3338,8 +3598,14 @@
         <f>out!F8</f>
         <v>341</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F8" s="4">
+        <v>42.03389830508474</v>
+      </c>
+      <c r="G8" s="4">
+        <v>70.210467498603094</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" s="8">
         <v>2</v>
       </c>
@@ -3358,8 +3624,14 @@
         <f>out!F15</f>
         <v>362</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F9" s="4">
+        <v>41.83347838700319</v>
+      </c>
+      <c r="G9" s="4">
+        <v>72.088047577603703</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" s="8">
         <v>3</v>
       </c>
@@ -3378,6 +3650,108 @@
         <f>out!F22</f>
         <v>332</v>
       </c>
+      <c r="F10" s="4">
+        <v>38.324386503067487</v>
+      </c>
+      <c r="G10" s="4">
+        <v>58.684216832822088</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A11" s="8" t="s">
+        <v>86</v>
+      </c>
+      <c r="B11" s="8" t="s">
+        <v>80</v>
+      </c>
+      <c r="C11" s="4">
+        <f>_xlfn.STDEV.P(C2:C4)</f>
+        <v>20.82199691565522</v>
+      </c>
+      <c r="D11" s="4">
+        <f>_xlfn.STDEV.P(D2:D4)</f>
+        <v>2.6246692913372702</v>
+      </c>
+      <c r="E11" s="4">
+        <f>_xlfn.STDEV.P(E2:E4)</f>
+        <v>20.049937655763422</v>
+      </c>
+      <c r="F11" s="4">
+        <f t="shared" ref="F11:G11" si="2">_xlfn.STDEV.P(F2:F4)</f>
+        <v>3.9435534967620714E-2</v>
+      </c>
+      <c r="G11" s="4">
+        <f t="shared" si="2"/>
+        <v>2.5151707893144999</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A12" s="8" t="s">
+        <v>86</v>
+      </c>
+      <c r="B12" s="8" t="s">
+        <v>81</v>
+      </c>
+      <c r="C12" s="4">
+        <f>_xlfn.STDEV.P(C5:C7)</f>
+        <v>2.6246692913372702</v>
+      </c>
+      <c r="D12" s="4">
+        <f>_xlfn.STDEV.P(D5:D7)</f>
+        <v>12.918548250050733</v>
+      </c>
+      <c r="E12" s="4">
+        <f>_xlfn.STDEV.P(E5:E7)</f>
+        <v>31.026870075253587</v>
+      </c>
+      <c r="F12" s="4">
+        <f t="shared" ref="F12:G12" si="3">_xlfn.STDEV.P(F5:F7)</f>
+        <v>2.3618412748501523E-2</v>
+      </c>
+      <c r="G12" s="4">
+        <f t="shared" si="3"/>
+        <v>2.283558898773832</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A13" s="8" t="s">
+        <v>86</v>
+      </c>
+      <c r="B13" s="8" t="s">
+        <v>82</v>
+      </c>
+      <c r="C13" s="4">
+        <f>_xlfn.STDEV.P(C8:C10)</f>
+        <v>31.026870075253587</v>
+      </c>
+      <c r="D13" s="4">
+        <f>_xlfn.STDEV.P(D8:D10)</f>
+        <v>12.119772641798562</v>
+      </c>
+      <c r="E13" s="4">
+        <f>_xlfn.STDEV.P(E8:E10)</f>
+        <v>12.569805089976535</v>
+      </c>
+      <c r="F13" s="4">
+        <f t="shared" ref="F13:G13" si="4">_xlfn.STDEV.P(F8:F10)</f>
+        <v>1.7034074283549212</v>
+      </c>
+      <c r="G13" s="4">
+        <f t="shared" si="4"/>
+        <v>5.9258608375889139</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="D14" s="4"/>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="D15" s="4"/>
+    </row>
+    <row r="17" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D17" s="4"/>
+    </row>
+    <row r="18" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D18" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3385,12 +3759,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{85C3B83D-07F9-42CF-81B8-88F53D1E2659}">
-  <dimension ref="A1:E10"/>
+  <dimension ref="A1:G18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I25" sqref="I25"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N10" sqref="N10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3398,7 +3772,7 @@
     <col min="1" max="16384" width="8.88671875" style="8"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="21" t="s">
         <v>66</v>
       </c>
@@ -3414,8 +3788,14 @@
       <c r="E1" s="21" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F1" s="21" t="s">
+        <v>84</v>
+      </c>
+      <c r="G1" s="21" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="8">
         <v>1</v>
       </c>
@@ -3434,8 +3814,14 @@
         <f>out!E3</f>
         <v>2.2799999999999998</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F2" s="4">
+        <v>25.081389940867716</v>
+      </c>
+      <c r="G2" s="4">
+        <v>41.438818163172755</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" s="8">
         <v>2</v>
       </c>
@@ -3454,8 +3840,14 @@
         <f>out!E10</f>
         <v>2.61</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F3" s="4">
+        <v>25.025977140116694</v>
+      </c>
+      <c r="G3" s="4">
+        <v>40.319629836854681</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" s="8">
         <v>3</v>
       </c>
@@ -3474,8 +3866,14 @@
         <f>out!E17</f>
         <v>1.39</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F4" s="4">
+        <v>25.122205745043114</v>
+      </c>
+      <c r="G4" s="4">
+        <v>35.632516311846864</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" s="8">
         <v>1</v>
       </c>
@@ -3494,8 +3892,14 @@
         <f>out!E6</f>
         <v>0.91</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F5" s="4">
+        <v>22.027475130270012</v>
+      </c>
+      <c r="G5" s="4">
+        <v>43.686509816306121</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" s="8">
         <v>2</v>
       </c>
@@ -3514,8 +3918,14 @@
         <f>out!E13</f>
         <v>1.1200000000000001</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F6" s="4">
+        <v>22.0036790717419</v>
+      </c>
+      <c r="G6" s="4">
+        <v>47.032349220362029</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" s="8">
         <v>3</v>
       </c>
@@ -3534,8 +3944,14 @@
         <f>out!E20</f>
         <v>0.64</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F7" s="4">
+        <v>21.969909354265958</v>
+      </c>
+      <c r="G7" s="4">
+        <v>41.47743201569947</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" s="8">
         <v>1</v>
       </c>
@@ -3554,8 +3970,14 @@
         <f>out!E8</f>
         <v>1.52</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F8" s="4">
+        <v>42.03389830508474</v>
+      </c>
+      <c r="G8" s="4">
+        <v>70.210467498603094</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" s="8">
         <v>2</v>
       </c>
@@ -3574,8 +3996,14 @@
         <f>out!E15</f>
         <v>1.93</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F9" s="4">
+        <v>41.83347838700319</v>
+      </c>
+      <c r="G9" s="4">
+        <v>72.088047577603703</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" s="8">
         <v>3</v>
       </c>
@@ -3594,6 +4022,108 @@
         <f>out!E22</f>
         <v>0.98</v>
       </c>
+      <c r="F10" s="4">
+        <v>38.324386503067487</v>
+      </c>
+      <c r="G10" s="4">
+        <v>58.684216832822088</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A11" s="8" t="s">
+        <v>86</v>
+      </c>
+      <c r="B11" s="8" t="s">
+        <v>80</v>
+      </c>
+      <c r="C11" s="4">
+        <f>_xlfn.STDEV.P(C2:C4)</f>
+        <v>0.26398653164297781</v>
+      </c>
+      <c r="D11" s="4">
+        <f>_xlfn.STDEV.P(D2:D4)</f>
+        <v>0.22050447211388433</v>
+      </c>
+      <c r="E11" s="4">
+        <f>_xlfn.STDEV.P(E2:E4)</f>
+        <v>0.51525613910839441</v>
+      </c>
+      <c r="F11" s="4">
+        <f t="shared" ref="F11:G11" si="2">_xlfn.STDEV.P(F2:F4)</f>
+        <v>3.9435534967620714E-2</v>
+      </c>
+      <c r="G11" s="4">
+        <f t="shared" si="2"/>
+        <v>2.5151707893144999</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A12" s="8" t="s">
+        <v>86</v>
+      </c>
+      <c r="B12" s="8" t="s">
+        <v>81</v>
+      </c>
+      <c r="C12" s="4">
+        <f>_xlfn.STDEV.P(C5:C7)</f>
+        <v>0.22050447211388433</v>
+      </c>
+      <c r="D12" s="4">
+        <f>_xlfn.STDEV.P(D5:D7)</f>
+        <v>0.12710450643291726</v>
+      </c>
+      <c r="E12" s="4">
+        <f>_xlfn.STDEV.P(E5:E7)</f>
+        <v>0.19646882704388513</v>
+      </c>
+      <c r="F12" s="4">
+        <f t="shared" ref="F12:G12" si="3">_xlfn.STDEV.P(F5:F7)</f>
+        <v>2.3618412748501523E-2</v>
+      </c>
+      <c r="G12" s="4">
+        <f t="shared" si="3"/>
+        <v>2.283558898773832</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A13" s="8" t="s">
+        <v>86</v>
+      </c>
+      <c r="B13" s="8" t="s">
+        <v>82</v>
+      </c>
+      <c r="C13" s="4">
+        <f>_xlfn.STDEV.P(C8:C10)</f>
+        <v>0.19646882704388513</v>
+      </c>
+      <c r="D13" s="4">
+        <f>_xlfn.STDEV.P(D8:D10)</f>
+        <v>5.3124591501697516E-2</v>
+      </c>
+      <c r="E13" s="4">
+        <f>_xlfn.STDEV.P(E8:E10)</f>
+        <v>0.38904441334577178</v>
+      </c>
+      <c r="F13" s="4">
+        <f t="shared" ref="F13:G13" si="4">_xlfn.STDEV.P(F8:F10)</f>
+        <v>1.7034074283549212</v>
+      </c>
+      <c r="G13" s="4">
+        <f t="shared" si="4"/>
+        <v>5.9258608375889139</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="D14" s="4"/>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="D15" s="4"/>
+    </row>
+    <row r="17" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D17" s="4"/>
+    </row>
+    <row r="18" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D18" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
changed order of trials and updated gitignore
</commit_message>
<xml_diff>
--- a/out.xlsx
+++ b/out.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\uphjan2\Projects\screen-audit\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\joe\Projects\screen-audit\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EAD9A391-8CC3-42ED-8480-8C3224CFB2E4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02DB55B3-1FAA-4772-A95F-AA598E0968C7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-24120" yWindow="-120" windowWidth="24240" windowHeight="13140" tabRatio="500" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4740" yWindow="2955" windowWidth="21600" windowHeight="11385" tabRatio="500" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="out" sheetId="1" r:id="rId1"/>
@@ -428,7 +428,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -506,6 +506,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -897,21 +900,21 @@
       <selection activeCell="O22" sqref="O22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="5.6640625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="4.44140625" style="1" customWidth="1"/>
-    <col min="3" max="6" width="8.88671875" style="1"/>
+    <col min="1" max="1" width="5.7109375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="4.42578125" style="1" customWidth="1"/>
+    <col min="3" max="6" width="8.85546875" style="1"/>
     <col min="7" max="7" width="6" style="1" customWidth="1"/>
     <col min="8" max="8" width="14" style="1" customWidth="1"/>
-    <col min="9" max="9" width="10.44140625" style="1" customWidth="1"/>
-    <col min="10" max="17" width="8.88671875" style="1"/>
-    <col min="18" max="18" width="9.88671875" style="1" customWidth="1"/>
-    <col min="19" max="19" width="11.77734375" style="1" customWidth="1"/>
-    <col min="20" max="1024" width="8.88671875" style="1"/>
+    <col min="9" max="9" width="10.42578125" style="1" customWidth="1"/>
+    <col min="10" max="17" width="8.85546875" style="1"/>
+    <col min="18" max="18" width="9.85546875" style="1" customWidth="1"/>
+    <col min="19" max="19" width="11.7109375" style="1" customWidth="1"/>
+    <col min="20" max="1024" width="8.85546875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:20" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
@@ -967,7 +970,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -1013,7 +1016,7 @@
         <v>0.58377811736392571</v>
       </c>
     </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -1054,7 +1057,7 @@
       </c>
       <c r="M3" s="5"/>
     </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -1087,7 +1090,7 @@
       </c>
       <c r="K4" s="4"/>
     </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>3</v>
       </c>
@@ -1129,7 +1132,7 @@
       </c>
       <c r="O5" s="5"/>
     </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>4</v>
       </c>
@@ -1162,7 +1165,7 @@
       </c>
       <c r="K6" s="4"/>
     </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>5</v>
       </c>
@@ -1195,7 +1198,7 @@
       </c>
       <c r="K7" s="4"/>
     </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A8" s="9">
         <v>6</v>
       </c>
@@ -1239,7 +1242,7 @@
         <v>0.70210467498603091</v>
       </c>
     </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>7</v>
       </c>
@@ -1284,7 +1287,7 @@
         <v>0.58628193198216028</v>
       </c>
     </row>
-    <row r="10" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>8</v>
       </c>
@@ -1325,7 +1328,7 @@
       </c>
       <c r="M10" s="5"/>
     </row>
-    <row r="11" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>9</v>
       </c>
@@ -1358,7 +1361,7 @@
       </c>
       <c r="K11" s="4"/>
     </row>
-    <row r="12" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>10</v>
       </c>
@@ -1400,7 +1403,7 @@
       </c>
       <c r="O12" s="5"/>
     </row>
-    <row r="13" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>11</v>
       </c>
@@ -1433,7 +1436,7 @@
       </c>
       <c r="K13" s="4"/>
     </row>
-    <row r="14" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>12</v>
       </c>
@@ -1466,7 +1469,7 @@
       </c>
       <c r="K14" s="4"/>
     </row>
-    <row r="15" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A15" s="9">
         <v>13</v>
       </c>
@@ -1510,7 +1513,7 @@
         <v>0.72088047577603709</v>
       </c>
     </row>
-    <row r="16" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>14</v>
       </c>
@@ -1555,7 +1558,7 @@
         <v>0.50271574549521014</v>
       </c>
     </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>15</v>
       </c>
@@ -1596,7 +1599,7 @@
       </c>
       <c r="M17" s="5"/>
     </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>16</v>
       </c>
@@ -1629,7 +1632,7 @@
       </c>
       <c r="K18" s="4"/>
     </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>17</v>
       </c>
@@ -1671,7 +1674,7 @@
       </c>
       <c r="O19" s="5"/>
     </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>18</v>
       </c>
@@ -1704,7 +1707,7 @@
       </c>
       <c r="K20" s="4"/>
     </row>
-    <row r="21" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>19</v>
       </c>
@@ -1737,7 +1740,7 @@
       </c>
       <c r="K21" s="4"/>
     </row>
-    <row r="22" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>20</v>
       </c>
@@ -1778,19 +1781,19 @@
         <v>0.58684216832822089</v>
       </c>
     </row>
-    <row r="24" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:16" x14ac:dyDescent="0.25">
       <c r="J24" s="20">
         <f>J2*3</f>
         <v>996.9782399999998</v>
       </c>
     </row>
-    <row r="25" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:16" x14ac:dyDescent="0.25">
       <c r="J25" s="20">
         <f>J9*3</f>
         <v>972.85536000000002</v>
       </c>
     </row>
-    <row r="26" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:16" x14ac:dyDescent="0.25">
       <c r="J26" s="20">
         <f>J16*3</f>
         <v>856.45728000000008</v>
@@ -1810,18 +1813,18 @@
       <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="4.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.88671875" style="1" customWidth="1"/>
-    <col min="4" max="4" width="10.21875" style="1" customWidth="1"/>
-    <col min="5" max="5" width="4.77734375" style="1" customWidth="1"/>
-    <col min="6" max="6" width="6.21875" style="1" customWidth="1"/>
-    <col min="7" max="7" width="5.109375" style="1" customWidth="1"/>
-    <col min="8" max="8" width="8.88671875" style="1"/>
+    <col min="2" max="2" width="4.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.85546875" style="1" customWidth="1"/>
+    <col min="4" max="4" width="10.28515625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="4.7109375" style="1" customWidth="1"/>
+    <col min="6" max="6" width="6.28515625" style="1" customWidth="1"/>
+    <col min="7" max="7" width="5.140625" style="1" customWidth="1"/>
+    <col min="8" max="8" width="8.85546875" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B2" s="21"/>
       <c r="C2" s="21" t="s">
         <v>89</v>
@@ -1835,7 +1838,7 @@
       <c r="F2" s="26"/>
       <c r="G2" s="26"/>
     </row>
-    <row r="3" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B3" s="22" t="s">
         <v>66</v>
       </c>
@@ -1855,7 +1858,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="4" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B4" s="1">
         <v>1</v>
       </c>
@@ -1875,7 +1878,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="5" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B5" s="1">
         <v>2</v>
       </c>
@@ -1895,7 +1898,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="6" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B6" s="1">
         <v>3</v>
       </c>
@@ -1932,13 +1935,13 @@
       <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="14" customWidth="1"/>
-    <col min="2" max="2" width="10.44140625" customWidth="1"/>
+    <col min="2" max="2" width="10.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>6</v>
       </c>
@@ -2012,7 +2015,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="2" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>20</v>
       </c>
@@ -2046,7 +2049,7 @@
       <c r="S2" s="1"/>
       <c r="T2" s="1"/>
     </row>
-    <row r="3" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>24</v>
       </c>
@@ -2080,7 +2083,7 @@
       <c r="S3" s="1"/>
       <c r="T3" s="1"/>
     </row>
-    <row r="4" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>28</v>
       </c>
@@ -2132,7 +2135,7 @@
       <c r="S4" s="1"/>
       <c r="T4" s="1"/>
     </row>
-    <row r="5" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>32</v>
       </c>
@@ -2182,7 +2185,7 @@
       <c r="S5" s="5"/>
       <c r="T5" s="1"/>
     </row>
-    <row r="6" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>36</v>
       </c>
@@ -2216,7 +2219,7 @@
       <c r="S6" s="1"/>
       <c r="T6" s="1"/>
     </row>
-    <row r="7" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>40</v>
       </c>
@@ -2250,7 +2253,7 @@
       <c r="S7" s="1"/>
       <c r="T7" s="1"/>
     </row>
-    <row r="8" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A8" s="9" t="s">
         <v>44</v>
       </c>
@@ -2304,7 +2307,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="9" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>20</v>
       </c>
@@ -2338,7 +2341,7 @@
       <c r="S9" s="1"/>
       <c r="T9" s="1"/>
     </row>
-    <row r="10" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>24</v>
       </c>
@@ -2372,7 +2375,7 @@
       <c r="S10" s="1"/>
       <c r="T10" s="1"/>
     </row>
-    <row r="11" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>28</v>
       </c>
@@ -2424,7 +2427,7 @@
       <c r="S11" s="1"/>
       <c r="T11" s="1"/>
     </row>
-    <row r="12" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>32</v>
       </c>
@@ -2474,7 +2477,7 @@
       <c r="S12" s="5"/>
       <c r="T12" s="1"/>
     </row>
-    <row r="13" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>36</v>
       </c>
@@ -2508,7 +2511,7 @@
       <c r="S13" s="1"/>
       <c r="T13" s="1"/>
     </row>
-    <row r="14" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>40</v>
       </c>
@@ -2542,7 +2545,7 @@
       <c r="S14" s="1"/>
       <c r="T14" s="1"/>
     </row>
-    <row r="15" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A15" s="9" t="s">
         <v>44</v>
       </c>
@@ -2596,7 +2599,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="16" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>20</v>
       </c>
@@ -2630,7 +2633,7 @@
       <c r="S16" s="1"/>
       <c r="T16" s="1"/>
     </row>
-    <row r="17" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>24</v>
       </c>
@@ -2664,7 +2667,7 @@
       <c r="S17" s="1"/>
       <c r="T17" s="1"/>
     </row>
-    <row r="18" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>28</v>
       </c>
@@ -2716,7 +2719,7 @@
       <c r="S18" s="1"/>
       <c r="T18" s="1"/>
     </row>
-    <row r="19" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>32</v>
       </c>
@@ -2766,7 +2769,7 @@
       <c r="S19" s="5"/>
       <c r="T19" s="1"/>
     </row>
-    <row r="20" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>36</v>
       </c>
@@ -2800,7 +2803,7 @@
       <c r="S20" s="1"/>
       <c r="T20" s="1"/>
     </row>
-    <row r="21" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>40</v>
       </c>
@@ -2834,7 +2837,7 @@
       <c r="S21" s="1"/>
       <c r="T21" s="1"/>
     </row>
-    <row r="22" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A22" s="9" t="s">
         <v>44</v>
       </c>
@@ -2900,20 +2903,20 @@
   <sheetViews>
     <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="3" width="8.6640625" style="1"/>
-    <col min="6" max="6" width="9.5546875" customWidth="1"/>
-    <col min="7" max="7" width="9.44140625" customWidth="1"/>
-    <col min="12" max="12" width="9.77734375" customWidth="1"/>
-    <col min="13" max="13" width="9.5546875" customWidth="1"/>
-    <col min="16" max="16" width="9.21875" customWidth="1"/>
-    <col min="18" max="18" width="9.77734375" customWidth="1"/>
-    <col min="19" max="19" width="9.5546875" customWidth="1"/>
-    <col min="1020" max="1024" width="11.5546875" customWidth="1"/>
+    <col min="1" max="3" width="8.7109375" style="1"/>
+    <col min="6" max="6" width="9.5703125" customWidth="1"/>
+    <col min="7" max="7" width="9.42578125" customWidth="1"/>
+    <col min="12" max="12" width="9.7109375" customWidth="1"/>
+    <col min="13" max="13" width="9.5703125" customWidth="1"/>
+    <col min="16" max="16" width="9.28515625" customWidth="1"/>
+    <col min="18" max="18" width="9.7109375" customWidth="1"/>
+    <col min="19" max="19" width="9.5703125" customWidth="1"/>
+    <col min="1020" max="1024" width="11.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A1" s="16" t="s">
         <v>66</v>
       </c>
@@ -2972,7 +2975,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -3031,7 +3034,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -3090,7 +3093,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -3149,7 +3152,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
       <c r="D5" s="1"/>
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
@@ -3163,7 +3166,7 @@
       <c r="N5" s="1"/>
       <c r="O5" s="1"/>
     </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
       <c r="D6" s="17"/>
       <c r="E6" s="17"/>
       <c r="F6" s="17"/>
@@ -3175,7 +3178,7 @@
       <c r="L6" s="17"/>
       <c r="M6" s="17"/>
     </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
       <c r="D7" s="1"/>
       <c r="E7" s="1"/>
       <c r="F7" s="1"/>
@@ -3189,7 +3192,7 @@
       <c r="N7" s="1"/>
       <c r="O7" s="1"/>
     </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
       <c r="D8" s="1"/>
       <c r="E8" s="1"/>
       <c r="F8" s="1"/>
@@ -3203,7 +3206,7 @@
       <c r="N8" s="1"/>
       <c r="O8" s="1"/>
     </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
       <c r="H9" s="1"/>
       <c r="I9" s="1"/>
       <c r="J9" s="1"/>
@@ -3213,7 +3216,7 @@
       <c r="N9" s="1"/>
       <c r="O9" s="1"/>
     </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
       <c r="D10" s="1"/>
       <c r="E10" s="1"/>
       <c r="F10" s="1"/>
@@ -3221,7 +3224,7 @@
       <c r="N10" s="5"/>
       <c r="O10" s="1"/>
     </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
       <c r="D11" s="1"/>
       <c r="E11" s="1"/>
       <c r="F11" s="1"/>
@@ -3235,7 +3238,7 @@
       <c r="N11" s="1"/>
       <c r="O11" s="1"/>
     </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
       <c r="D12" s="1"/>
       <c r="E12" s="1"/>
       <c r="F12" s="1"/>
@@ -3249,7 +3252,7 @@
       <c r="N12" s="1"/>
       <c r="O12" s="1"/>
     </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
       <c r="D13" s="17"/>
       <c r="E13" s="17"/>
       <c r="F13" s="17"/>
@@ -3261,7 +3264,7 @@
       <c r="L13" s="17"/>
       <c r="M13" s="17"/>
     </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
       <c r="D14" s="1"/>
       <c r="E14" s="1"/>
       <c r="F14" s="1"/>
@@ -3275,7 +3278,7 @@
       <c r="N14" s="1"/>
       <c r="O14" s="1"/>
     </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
       <c r="D15" s="1"/>
       <c r="E15" s="1"/>
       <c r="F15" s="1"/>
@@ -3289,7 +3292,7 @@
       <c r="N15" s="1"/>
       <c r="O15" s="1"/>
     </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
       <c r="H16" s="1"/>
       <c r="I16" s="1"/>
       <c r="J16" s="1"/>
@@ -3299,7 +3302,7 @@
       <c r="N16" s="1"/>
       <c r="O16" s="1"/>
     </row>
-    <row r="17" spans="4:15" x14ac:dyDescent="0.3">
+    <row r="17" spans="4:15" x14ac:dyDescent="0.25">
       <c r="D17" s="1"/>
       <c r="E17" s="1"/>
       <c r="F17" s="1"/>
@@ -3307,7 +3310,7 @@
       <c r="N17" s="5"/>
       <c r="O17" s="1"/>
     </row>
-    <row r="18" spans="4:15" x14ac:dyDescent="0.3">
+    <row r="18" spans="4:15" x14ac:dyDescent="0.25">
       <c r="D18" s="1"/>
       <c r="E18" s="1"/>
       <c r="F18" s="1"/>
@@ -3321,7 +3324,7 @@
       <c r="N18" s="1"/>
       <c r="O18" s="1"/>
     </row>
-    <row r="19" spans="4:15" x14ac:dyDescent="0.3">
+    <row r="19" spans="4:15" x14ac:dyDescent="0.25">
       <c r="D19" s="1"/>
       <c r="E19" s="1"/>
       <c r="F19" s="1"/>
@@ -3335,7 +3338,7 @@
       <c r="N19" s="1"/>
       <c r="O19" s="1"/>
     </row>
-    <row r="20" spans="4:15" x14ac:dyDescent="0.3">
+    <row r="20" spans="4:15" x14ac:dyDescent="0.25">
       <c r="D20" s="17"/>
       <c r="E20" s="17"/>
       <c r="F20" s="17"/>
@@ -3365,13 +3368,13 @@
       <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="9.109375" customWidth="1"/>
-    <col min="4" max="5" width="8.88671875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="9.140625" customWidth="1"/>
+    <col min="4" max="5" width="8.85546875" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>66</v>
       </c>
@@ -3388,7 +3391,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -3407,7 +3410,7 @@
       <c r="G2" s="4"/>
       <c r="H2" s="4"/>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -3426,7 +3429,7 @@
       <c r="G3" s="4"/>
       <c r="H3" s="4"/>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -3445,7 +3448,7 @@
       <c r="G4" s="4"/>
       <c r="H4" s="4"/>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>1</v>
       </c>
@@ -3464,7 +3467,7 @@
       <c r="G5" s="4"/>
       <c r="H5" s="4"/>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>2</v>
       </c>
@@ -3483,7 +3486,7 @@
       <c r="G6" s="4"/>
       <c r="H6" s="4"/>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>3</v>
       </c>
@@ -3502,7 +3505,7 @@
       <c r="G7" s="4"/>
       <c r="H7" s="4"/>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>1</v>
       </c>
@@ -3521,7 +3524,7 @@
       <c r="G8" s="4"/>
       <c r="H8" s="4"/>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>2</v>
       </c>
@@ -3540,7 +3543,7 @@
       <c r="G9" s="4"/>
       <c r="H9" s="4"/>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>3</v>
       </c>
@@ -3569,18 +3572,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:AMJ18"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="5" width="8.88671875" style="1"/>
-    <col min="6" max="7" width="9.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="1024" width="8.88671875" style="1"/>
+    <col min="1" max="5" width="8.85546875" style="1"/>
+    <col min="6" max="7" width="9.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="1024" width="8.85546875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>66</v>
       </c>
@@ -3603,7 +3606,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -3629,7 +3632,7 @@
         <v>41.438818163172797</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -3655,7 +3658,7 @@
         <v>40.319629836854702</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -3681,7 +3684,7 @@
         <v>35.632516311846899</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>1</v>
       </c>
@@ -3707,7 +3710,7 @@
         <v>43.686509816306099</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>2</v>
       </c>
@@ -3733,7 +3736,7 @@
         <v>47.032349220362001</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>3</v>
       </c>
@@ -3759,7 +3762,7 @@
         <v>41.477432015699499</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>1</v>
       </c>
@@ -3785,7 +3788,7 @@
         <v>70.210467498603094</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>2</v>
       </c>
@@ -3811,7 +3814,7 @@
         <v>72.088047577603703</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>3</v>
       </c>
@@ -3837,7 +3840,7 @@
         <v>58.684216832822102</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>86</v>
       </c>
@@ -3865,7 +3868,7 @@
         <v>2.5151707893144999</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>86</v>
       </c>
@@ -3893,7 +3896,7 @@
         <v>2.2835588987738102</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>86</v>
       </c>
@@ -3921,7 +3924,7 @@
         <v>5.9258608375889077</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>1</v>
       </c>
@@ -3947,7 +3950,7 @@
         <v>59.400998287645145</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>2</v>
       </c>
@@ -3973,7 +3976,7 @@
         <v>60.554081661965562</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>3</v>
       </c>
@@ -3999,10 +4002,10 @@
         <v>51.300016366594406</v>
       </c>
     </row>
-    <row r="17" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="17" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D17" s="4"/>
     </row>
-    <row r="18" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="18" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D18" s="4"/>
     </row>
   </sheetData>
@@ -4015,20 +4018,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:AMJ18"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F21" sqref="F21"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I17" sqref="I17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.88671875" style="1"/>
-    <col min="2" max="2" width="10.21875" style="1" customWidth="1"/>
-    <col min="3" max="17" width="8.88671875" style="1"/>
-    <col min="18" max="18" width="17.109375" style="1" customWidth="1"/>
-    <col min="19" max="1024" width="8.88671875" style="1"/>
+    <col min="1" max="1" width="8.85546875" style="1"/>
+    <col min="2" max="2" width="10.28515625" style="1" customWidth="1"/>
+    <col min="3" max="17" width="8.85546875" style="1"/>
+    <col min="18" max="18" width="17.140625" style="1" customWidth="1"/>
+    <col min="19" max="1024" width="8.85546875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>66</v>
       </c>
@@ -4054,7 +4057,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -4082,7 +4085,7 @@
       <c r="H2"/>
       <c r="R2" s="4"/>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -4110,7 +4113,7 @@
       <c r="H3"/>
       <c r="R3" s="4"/>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -4138,7 +4141,7 @@
       <c r="H4"/>
       <c r="R4" s="4"/>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>1</v>
       </c>
@@ -4164,7 +4167,7 @@
         <v>43.686509816306099</v>
       </c>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>2</v>
       </c>
@@ -4190,7 +4193,7 @@
         <v>47.032349220362001</v>
       </c>
     </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>3</v>
       </c>
@@ -4216,7 +4219,7 @@
         <v>41.477432015699499</v>
       </c>
     </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>1</v>
       </c>
@@ -4242,7 +4245,7 @@
         <v>70.210467498603094</v>
       </c>
     </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>2</v>
       </c>
@@ -4268,7 +4271,7 @@
         <v>72.088047577603703</v>
       </c>
     </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>3</v>
       </c>
@@ -4294,7 +4297,7 @@
         <v>58.684216832822102</v>
       </c>
     </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>86</v>
       </c>
@@ -4322,7 +4325,7 @@
         <v>2.5151707893144999</v>
       </c>
     </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>86</v>
       </c>
@@ -4350,7 +4353,7 @@
         <v>2.2835588987738102</v>
       </c>
     </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>86</v>
       </c>
@@ -4378,7 +4381,7 @@
         <v>5.9258608375889077</v>
       </c>
     </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>1</v>
       </c>
@@ -4389,12 +4392,19 @@
         <f>C2</f>
         <v>1.38</v>
       </c>
-      <c r="D14" s="4"/>
+      <c r="D14" s="4">
+        <f>AVERAGE(D5,D8)</f>
+        <v>0.62</v>
+      </c>
+      <c r="E14" s="27">
+        <f>AVERAGE(E2,E8)</f>
+        <v>1.9</v>
+      </c>
       <c r="G14" s="4">
         <v>59.400998287645102</v>
       </c>
     </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>2</v>
       </c>
@@ -4405,12 +4415,19 @@
         <f>C3</f>
         <v>1.62</v>
       </c>
-      <c r="D15" s="4"/>
+      <c r="D15" s="4">
+        <f t="shared" ref="D15:D16" si="0">AVERAGE(D6,D9)</f>
+        <v>0.71500000000000008</v>
+      </c>
+      <c r="E15" s="27">
+        <f t="shared" ref="E15:E16" si="1">AVERAGE(E3,E9)</f>
+        <v>2.27</v>
+      </c>
       <c r="G15" s="4">
         <v>60.554081661965597</v>
       </c>
     </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>3</v>
       </c>
@@ -4421,14 +4438,22 @@
         <f>C4</f>
         <v>0.98</v>
       </c>
+      <c r="D16" s="4">
+        <f t="shared" si="0"/>
+        <v>0.495</v>
+      </c>
+      <c r="E16" s="27">
+        <f t="shared" si="1"/>
+        <v>1.1850000000000001</v>
+      </c>
       <c r="G16" s="4">
         <v>51.300016366594399</v>
       </c>
     </row>
-    <row r="17" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="17" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D17" s="4"/>
     </row>
-    <row r="18" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="18" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D18" s="4"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
commit when issued email and ppt remote
</commit_message>
<xml_diff>
--- a/out.xlsx
+++ b/out.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\joe\Projects\screen-audit\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\uphjan2\Projects\screen-audit\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02DB55B3-1FAA-4772-A95F-AA598E0968C7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76606C53-6FA7-40C0-B3F8-FE269344121C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4740" yWindow="2955" windowWidth="21600" windowHeight="11385" tabRatio="500" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-24120" yWindow="-120" windowWidth="24240" windowHeight="13140" tabRatio="500" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="out" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="261" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="261" uniqueCount="94">
   <si>
     <t>trial</t>
   </si>
@@ -321,9 +321,6 @@
   </si>
   <si>
     <t>%</t>
-  </si>
-  <si>
-    <t>FPS</t>
   </si>
 </sst>
 </file>
@@ -505,10 +502,10 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -897,24 +894,24 @@
   <dimension ref="A1:AMJ26"/>
   <sheetViews>
     <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="O22" sqref="O22"/>
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="5.7109375" style="1" customWidth="1"/>
-    <col min="2" max="2" width="4.42578125" style="1" customWidth="1"/>
-    <col min="3" max="6" width="8.85546875" style="1"/>
+    <col min="1" max="1" width="5.6640625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="4.44140625" style="1" customWidth="1"/>
+    <col min="3" max="6" width="8.88671875" style="1"/>
     <col min="7" max="7" width="6" style="1" customWidth="1"/>
     <col min="8" max="8" width="14" style="1" customWidth="1"/>
-    <col min="9" max="9" width="10.42578125" style="1" customWidth="1"/>
-    <col min="10" max="17" width="8.85546875" style="1"/>
-    <col min="18" max="18" width="9.85546875" style="1" customWidth="1"/>
-    <col min="19" max="19" width="11.7109375" style="1" customWidth="1"/>
-    <col min="20" max="1024" width="8.85546875" style="1"/>
+    <col min="9" max="9" width="10.44140625" style="1" customWidth="1"/>
+    <col min="10" max="17" width="8.88671875" style="1"/>
+    <col min="18" max="18" width="9.88671875" style="1" customWidth="1"/>
+    <col min="19" max="19" width="11.6640625" style="1" customWidth="1"/>
+    <col min="20" max="1024" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:20" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
@@ -970,7 +967,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -1016,7 +1013,7 @@
         <v>0.58377811736392571</v>
       </c>
     </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -1057,7 +1054,7 @@
       </c>
       <c r="M3" s="5"/>
     </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -1090,7 +1087,7 @@
       </c>
       <c r="K4" s="4"/>
     </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
         <v>3</v>
       </c>
@@ -1132,7 +1129,7 @@
       </c>
       <c r="O5" s="5"/>
     </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
         <v>4</v>
       </c>
@@ -1165,7 +1162,7 @@
       </c>
       <c r="K6" s="4"/>
     </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
         <v>5</v>
       </c>
@@ -1198,7 +1195,7 @@
       </c>
       <c r="K7" s="4"/>
     </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A8" s="9">
         <v>6</v>
       </c>
@@ -1242,7 +1239,7 @@
         <v>0.70210467498603091</v>
       </c>
     </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
         <v>7</v>
       </c>
@@ -1287,7 +1284,7 @@
         <v>0.58628193198216028</v>
       </c>
     </row>
-    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
         <v>8</v>
       </c>
@@ -1328,7 +1325,7 @@
       </c>
       <c r="M10" s="5"/>
     </row>
-    <row r="11" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A11" s="1">
         <v>9</v>
       </c>
@@ -1361,7 +1358,7 @@
       </c>
       <c r="K11" s="4"/>
     </row>
-    <row r="12" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A12" s="1">
         <v>10</v>
       </c>
@@ -1403,7 +1400,7 @@
       </c>
       <c r="O12" s="5"/>
     </row>
-    <row r="13" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A13" s="1">
         <v>11</v>
       </c>
@@ -1436,7 +1433,7 @@
       </c>
       <c r="K13" s="4"/>
     </row>
-    <row r="14" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A14" s="1">
         <v>12</v>
       </c>
@@ -1469,7 +1466,7 @@
       </c>
       <c r="K14" s="4"/>
     </row>
-    <row r="15" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A15" s="9">
         <v>13</v>
       </c>
@@ -1513,7 +1510,7 @@
         <v>0.72088047577603709</v>
       </c>
     </row>
-    <row r="16" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A16" s="1">
         <v>14</v>
       </c>
@@ -1558,7 +1555,7 @@
         <v>0.50271574549521014</v>
       </c>
     </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A17" s="1">
         <v>15</v>
       </c>
@@ -1599,7 +1596,7 @@
       </c>
       <c r="M17" s="5"/>
     </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A18" s="1">
         <v>16</v>
       </c>
@@ -1632,7 +1629,7 @@
       </c>
       <c r="K18" s="4"/>
     </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A19" s="1">
         <v>17</v>
       </c>
@@ -1674,7 +1671,7 @@
       </c>
       <c r="O19" s="5"/>
     </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A20" s="1">
         <v>18</v>
       </c>
@@ -1707,7 +1704,7 @@
       </c>
       <c r="K20" s="4"/>
     </row>
-    <row r="21" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A21" s="1">
         <v>19</v>
       </c>
@@ -1740,7 +1737,7 @@
       </c>
       <c r="K21" s="4"/>
     </row>
-    <row r="22" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A22" s="1">
         <v>20</v>
       </c>
@@ -1781,19 +1778,19 @@
         <v>0.58684216832822089</v>
       </c>
     </row>
-    <row r="24" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:16" x14ac:dyDescent="0.3">
       <c r="J24" s="20">
         <f>J2*3</f>
         <v>996.9782399999998</v>
       </c>
     </row>
-    <row r="25" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:16" x14ac:dyDescent="0.3">
       <c r="J25" s="20">
         <f>J9*3</f>
         <v>972.85536000000002</v>
       </c>
     </row>
-    <row r="26" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:16" x14ac:dyDescent="0.3">
       <c r="J26" s="20">
         <f>J16*3</f>
         <v>856.45728000000008</v>
@@ -1813,18 +1810,18 @@
       <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="4.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.85546875" style="1" customWidth="1"/>
-    <col min="4" max="4" width="10.28515625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="4.7109375" style="1" customWidth="1"/>
-    <col min="6" max="6" width="6.28515625" style="1" customWidth="1"/>
-    <col min="7" max="7" width="5.140625" style="1" customWidth="1"/>
-    <col min="8" max="8" width="8.85546875" style="1"/>
+    <col min="2" max="2" width="4.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.88671875" style="1" customWidth="1"/>
+    <col min="4" max="4" width="10.33203125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="4.6640625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="6.33203125" style="1" customWidth="1"/>
+    <col min="7" max="7" width="5.109375" style="1" customWidth="1"/>
+    <col min="8" max="8" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B2" s="21"/>
       <c r="C2" s="21" t="s">
         <v>89</v>
@@ -1832,13 +1829,13 @@
       <c r="D2" s="25" t="s">
         <v>90</v>
       </c>
-      <c r="E2" s="26" t="s">
+      <c r="E2" s="27" t="s">
         <v>91</v>
       </c>
-      <c r="F2" s="26"/>
-      <c r="G2" s="26"/>
-    </row>
-    <row r="3" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="F2" s="27"/>
+      <c r="G2" s="27"/>
+    </row>
+    <row r="3" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B3" s="22" t="s">
         <v>66</v>
       </c>
@@ -1858,7 +1855,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="4" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B4" s="1">
         <v>1</v>
       </c>
@@ -1878,7 +1875,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="5" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B5" s="1">
         <v>2</v>
       </c>
@@ -1898,7 +1895,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="6" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B6" s="1">
         <v>3</v>
       </c>
@@ -1935,13 +1932,13 @@
       <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="14" customWidth="1"/>
-    <col min="2" max="2" width="10.42578125" customWidth="1"/>
+    <col min="2" max="2" width="10.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>6</v>
       </c>
@@ -2015,7 +2012,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="2" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>20</v>
       </c>
@@ -2049,7 +2046,7 @@
       <c r="S2" s="1"/>
       <c r="T2" s="1"/>
     </row>
-    <row r="3" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>24</v>
       </c>
@@ -2083,7 +2080,7 @@
       <c r="S3" s="1"/>
       <c r="T3" s="1"/>
     </row>
-    <row r="4" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>28</v>
       </c>
@@ -2135,7 +2132,7 @@
       <c r="S4" s="1"/>
       <c r="T4" s="1"/>
     </row>
-    <row r="5" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>32</v>
       </c>
@@ -2185,7 +2182,7 @@
       <c r="S5" s="5"/>
       <c r="T5" s="1"/>
     </row>
-    <row r="6" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>36</v>
       </c>
@@ -2219,7 +2216,7 @@
       <c r="S6" s="1"/>
       <c r="T6" s="1"/>
     </row>
-    <row r="7" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>40</v>
       </c>
@@ -2253,7 +2250,7 @@
       <c r="S7" s="1"/>
       <c r="T7" s="1"/>
     </row>
-    <row r="8" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A8" s="9" t="s">
         <v>44</v>
       </c>
@@ -2307,7 +2304,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="9" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>20</v>
       </c>
@@ -2341,7 +2338,7 @@
       <c r="S9" s="1"/>
       <c r="T9" s="1"/>
     </row>
-    <row r="10" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>24</v>
       </c>
@@ -2375,7 +2372,7 @@
       <c r="S10" s="1"/>
       <c r="T10" s="1"/>
     </row>
-    <row r="11" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>28</v>
       </c>
@@ -2427,7 +2424,7 @@
       <c r="S11" s="1"/>
       <c r="T11" s="1"/>
     </row>
-    <row r="12" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>32</v>
       </c>
@@ -2477,7 +2474,7 @@
       <c r="S12" s="5"/>
       <c r="T12" s="1"/>
     </row>
-    <row r="13" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>36</v>
       </c>
@@ -2511,7 +2508,7 @@
       <c r="S13" s="1"/>
       <c r="T13" s="1"/>
     </row>
-    <row r="14" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>40</v>
       </c>
@@ -2545,7 +2542,7 @@
       <c r="S14" s="1"/>
       <c r="T14" s="1"/>
     </row>
-    <row r="15" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A15" s="9" t="s">
         <v>44</v>
       </c>
@@ -2599,7 +2596,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="16" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
         <v>20</v>
       </c>
@@ -2633,7 +2630,7 @@
       <c r="S16" s="1"/>
       <c r="T16" s="1"/>
     </row>
-    <row r="17" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
         <v>24</v>
       </c>
@@ -2667,7 +2664,7 @@
       <c r="S17" s="1"/>
       <c r="T17" s="1"/>
     </row>
-    <row r="18" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
         <v>28</v>
       </c>
@@ -2719,7 +2716,7 @@
       <c r="S18" s="1"/>
       <c r="T18" s="1"/>
     </row>
-    <row r="19" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
         <v>32</v>
       </c>
@@ -2769,7 +2766,7 @@
       <c r="S19" s="5"/>
       <c r="T19" s="1"/>
     </row>
-    <row r="20" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
         <v>36</v>
       </c>
@@ -2803,7 +2800,7 @@
       <c r="S20" s="1"/>
       <c r="T20" s="1"/>
     </row>
-    <row r="21" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
         <v>40</v>
       </c>
@@ -2837,7 +2834,7 @@
       <c r="S21" s="1"/>
       <c r="T21" s="1"/>
     </row>
-    <row r="22" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A22" s="9" t="s">
         <v>44</v>
       </c>
@@ -2903,20 +2900,20 @@
   <sheetViews>
     <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="3" width="8.7109375" style="1"/>
-    <col min="6" max="6" width="9.5703125" customWidth="1"/>
-    <col min="7" max="7" width="9.42578125" customWidth="1"/>
-    <col min="12" max="12" width="9.7109375" customWidth="1"/>
-    <col min="13" max="13" width="9.5703125" customWidth="1"/>
-    <col min="16" max="16" width="9.28515625" customWidth="1"/>
-    <col min="18" max="18" width="9.7109375" customWidth="1"/>
-    <col min="19" max="19" width="9.5703125" customWidth="1"/>
-    <col min="1020" max="1024" width="11.5703125" customWidth="1"/>
+    <col min="1" max="3" width="8.6640625" style="1"/>
+    <col min="6" max="6" width="9.5546875" customWidth="1"/>
+    <col min="7" max="7" width="9.44140625" customWidth="1"/>
+    <col min="12" max="12" width="9.6640625" customWidth="1"/>
+    <col min="13" max="13" width="9.5546875" customWidth="1"/>
+    <col min="16" max="16" width="9.33203125" customWidth="1"/>
+    <col min="18" max="18" width="9.6640625" customWidth="1"/>
+    <col min="19" max="19" width="9.5546875" customWidth="1"/>
+    <col min="1020" max="1024" width="11.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A1" s="16" t="s">
         <v>66</v>
       </c>
@@ -2975,7 +2972,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -3034,7 +3031,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -3093,7 +3090,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -3152,7 +3149,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:19" x14ac:dyDescent="0.3">
       <c r="D5" s="1"/>
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
@@ -3166,7 +3163,7 @@
       <c r="N5" s="1"/>
       <c r="O5" s="1"/>
     </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:19" x14ac:dyDescent="0.3">
       <c r="D6" s="17"/>
       <c r="E6" s="17"/>
       <c r="F6" s="17"/>
@@ -3178,7 +3175,7 @@
       <c r="L6" s="17"/>
       <c r="M6" s="17"/>
     </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:19" x14ac:dyDescent="0.3">
       <c r="D7" s="1"/>
       <c r="E7" s="1"/>
       <c r="F7" s="1"/>
@@ -3192,7 +3189,7 @@
       <c r="N7" s="1"/>
       <c r="O7" s="1"/>
     </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:19" x14ac:dyDescent="0.3">
       <c r="D8" s="1"/>
       <c r="E8" s="1"/>
       <c r="F8" s="1"/>
@@ -3206,7 +3203,7 @@
       <c r="N8" s="1"/>
       <c r="O8" s="1"/>
     </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:19" x14ac:dyDescent="0.3">
       <c r="H9" s="1"/>
       <c r="I9" s="1"/>
       <c r="J9" s="1"/>
@@ -3216,7 +3213,7 @@
       <c r="N9" s="1"/>
       <c r="O9" s="1"/>
     </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:19" x14ac:dyDescent="0.3">
       <c r="D10" s="1"/>
       <c r="E10" s="1"/>
       <c r="F10" s="1"/>
@@ -3224,7 +3221,7 @@
       <c r="N10" s="5"/>
       <c r="O10" s="1"/>
     </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:19" x14ac:dyDescent="0.3">
       <c r="D11" s="1"/>
       <c r="E11" s="1"/>
       <c r="F11" s="1"/>
@@ -3238,7 +3235,7 @@
       <c r="N11" s="1"/>
       <c r="O11" s="1"/>
     </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:19" x14ac:dyDescent="0.3">
       <c r="D12" s="1"/>
       <c r="E12" s="1"/>
       <c r="F12" s="1"/>
@@ -3252,7 +3249,7 @@
       <c r="N12" s="1"/>
       <c r="O12" s="1"/>
     </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:19" x14ac:dyDescent="0.3">
       <c r="D13" s="17"/>
       <c r="E13" s="17"/>
       <c r="F13" s="17"/>
@@ -3264,7 +3261,7 @@
       <c r="L13" s="17"/>
       <c r="M13" s="17"/>
     </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:19" x14ac:dyDescent="0.3">
       <c r="D14" s="1"/>
       <c r="E14" s="1"/>
       <c r="F14" s="1"/>
@@ -3278,7 +3275,7 @@
       <c r="N14" s="1"/>
       <c r="O14" s="1"/>
     </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:19" x14ac:dyDescent="0.3">
       <c r="D15" s="1"/>
       <c r="E15" s="1"/>
       <c r="F15" s="1"/>
@@ -3292,7 +3289,7 @@
       <c r="N15" s="1"/>
       <c r="O15" s="1"/>
     </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:19" x14ac:dyDescent="0.3">
       <c r="H16" s="1"/>
       <c r="I16" s="1"/>
       <c r="J16" s="1"/>
@@ -3302,7 +3299,7 @@
       <c r="N16" s="1"/>
       <c r="O16" s="1"/>
     </row>
-    <row r="17" spans="4:15" x14ac:dyDescent="0.25">
+    <row r="17" spans="4:15" x14ac:dyDescent="0.3">
       <c r="D17" s="1"/>
       <c r="E17" s="1"/>
       <c r="F17" s="1"/>
@@ -3310,7 +3307,7 @@
       <c r="N17" s="5"/>
       <c r="O17" s="1"/>
     </row>
-    <row r="18" spans="4:15" x14ac:dyDescent="0.25">
+    <row r="18" spans="4:15" x14ac:dyDescent="0.3">
       <c r="D18" s="1"/>
       <c r="E18" s="1"/>
       <c r="F18" s="1"/>
@@ -3324,7 +3321,7 @@
       <c r="N18" s="1"/>
       <c r="O18" s="1"/>
     </row>
-    <row r="19" spans="4:15" x14ac:dyDescent="0.25">
+    <row r="19" spans="4:15" x14ac:dyDescent="0.3">
       <c r="D19" s="1"/>
       <c r="E19" s="1"/>
       <c r="F19" s="1"/>
@@ -3338,7 +3335,7 @@
       <c r="N19" s="1"/>
       <c r="O19" s="1"/>
     </row>
-    <row r="20" spans="4:15" x14ac:dyDescent="0.25">
+    <row r="20" spans="4:15" x14ac:dyDescent="0.3">
       <c r="D20" s="17"/>
       <c r="E20" s="17"/>
       <c r="F20" s="17"/>
@@ -3368,13 +3365,13 @@
       <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="3" width="9.140625" customWidth="1"/>
-    <col min="4" max="5" width="8.85546875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="9.109375" customWidth="1"/>
+    <col min="4" max="5" width="8.88671875" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>66</v>
       </c>
@@ -3391,7 +3388,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -3410,7 +3407,7 @@
       <c r="G2" s="4"/>
       <c r="H2" s="4"/>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -3429,7 +3426,7 @@
       <c r="G3" s="4"/>
       <c r="H3" s="4"/>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -3448,7 +3445,7 @@
       <c r="G4" s="4"/>
       <c r="H4" s="4"/>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
         <v>1</v>
       </c>
@@ -3467,7 +3464,7 @@
       <c r="G5" s="4"/>
       <c r="H5" s="4"/>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
         <v>2</v>
       </c>
@@ -3486,7 +3483,7 @@
       <c r="G6" s="4"/>
       <c r="H6" s="4"/>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
         <v>3</v>
       </c>
@@ -3505,7 +3502,7 @@
       <c r="G7" s="4"/>
       <c r="H7" s="4"/>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
         <v>1</v>
       </c>
@@ -3524,7 +3521,7 @@
       <c r="G8" s="4"/>
       <c r="H8" s="4"/>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
         <v>2</v>
       </c>
@@ -3543,7 +3540,7 @@
       <c r="G9" s="4"/>
       <c r="H9" s="4"/>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
         <v>3</v>
       </c>
@@ -3573,17 +3570,19 @@
   <dimension ref="A1:AMJ18"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E24" sqref="E24"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="5" width="8.85546875" style="1"/>
-    <col min="6" max="7" width="9.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="1024" width="8.85546875" style="1"/>
+    <col min="1" max="1" width="8.88671875" style="1"/>
+    <col min="2" max="2" width="9.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="5" width="8.88671875" style="1"/>
+    <col min="6" max="7" width="9.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="1024" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>66</v>
       </c>
@@ -3606,7 +3605,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -3632,7 +3631,7 @@
         <v>41.438818163172797</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -3658,7 +3657,7 @@
         <v>40.319629836854702</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -3684,7 +3683,7 @@
         <v>35.632516311846899</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
         <v>1</v>
       </c>
@@ -3710,7 +3709,7 @@
         <v>43.686509816306099</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
         <v>2</v>
       </c>
@@ -3736,7 +3735,7 @@
         <v>47.032349220362001</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
         <v>3</v>
       </c>
@@ -3762,7 +3761,7 @@
         <v>41.477432015699499</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
         <v>1</v>
       </c>
@@ -3788,7 +3787,7 @@
         <v>70.210467498603094</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
         <v>2</v>
       </c>
@@ -3814,7 +3813,7 @@
         <v>72.088047577603703</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
         <v>3</v>
       </c>
@@ -3840,7 +3839,7 @@
         <v>58.684216832822102</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>86</v>
       </c>
@@ -3868,7 +3867,7 @@
         <v>2.5151707893144999</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>86</v>
       </c>
@@ -3896,7 +3895,7 @@
         <v>2.2835588987738102</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>86</v>
       </c>
@@ -3924,12 +3923,12 @@
         <v>5.9258608375889077</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" s="1">
         <v>1</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="C14" s="1">
         <f>C2</f>
@@ -3950,12 +3949,12 @@
         <v>59.400998287645145</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" s="1">
         <v>2</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="C15" s="1">
         <f t="shared" ref="C15:C16" si="0">C3</f>
@@ -3976,12 +3975,12 @@
         <v>60.554081661965562</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" s="1">
         <v>3</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="C16" s="1">
         <f t="shared" si="0"/>
@@ -4002,10 +4001,10 @@
         <v>51.300016366594406</v>
       </c>
     </row>
-    <row r="17" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D17" s="4"/>
     </row>
-    <row r="18" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D18" s="4"/>
     </row>
   </sheetData>
@@ -4019,19 +4018,19 @@
   <dimension ref="A1:AMJ18"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I17" sqref="I17"/>
+      <selection activeCell="G21" sqref="G21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="8.85546875" style="1"/>
-    <col min="2" max="2" width="10.28515625" style="1" customWidth="1"/>
-    <col min="3" max="17" width="8.85546875" style="1"/>
-    <col min="18" max="18" width="17.140625" style="1" customWidth="1"/>
-    <col min="19" max="1024" width="8.85546875" style="1"/>
+    <col min="1" max="1" width="8.88671875" style="1"/>
+    <col min="2" max="2" width="10.33203125" style="1" customWidth="1"/>
+    <col min="3" max="17" width="8.88671875" style="1"/>
+    <col min="18" max="18" width="17.109375" style="1" customWidth="1"/>
+    <col min="19" max="1024" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>66</v>
       </c>
@@ -4057,7 +4056,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -4085,7 +4084,7 @@
       <c r="H2"/>
       <c r="R2" s="4"/>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -4113,7 +4112,7 @@
       <c r="H3"/>
       <c r="R3" s="4"/>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -4141,7 +4140,7 @@
       <c r="H4"/>
       <c r="R4" s="4"/>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
         <v>1</v>
       </c>
@@ -4167,7 +4166,7 @@
         <v>43.686509816306099</v>
       </c>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
         <v>2</v>
       </c>
@@ -4193,7 +4192,7 @@
         <v>47.032349220362001</v>
       </c>
     </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
         <v>3</v>
       </c>
@@ -4219,7 +4218,7 @@
         <v>41.477432015699499</v>
       </c>
     </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
         <v>1</v>
       </c>
@@ -4245,7 +4244,7 @@
         <v>70.210467498603094</v>
       </c>
     </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
         <v>2</v>
       </c>
@@ -4271,7 +4270,7 @@
         <v>72.088047577603703</v>
       </c>
     </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
         <v>3</v>
       </c>
@@ -4297,7 +4296,7 @@
         <v>58.684216832822102</v>
       </c>
     </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>86</v>
       </c>
@@ -4325,7 +4324,7 @@
         <v>2.5151707893144999</v>
       </c>
     </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>86</v>
       </c>
@@ -4353,7 +4352,7 @@
         <v>2.2835588987738102</v>
       </c>
     </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>86</v>
       </c>
@@ -4381,7 +4380,7 @@
         <v>5.9258608375889077</v>
       </c>
     </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A14" s="1">
         <v>1</v>
       </c>
@@ -4396,7 +4395,7 @@
         <f>AVERAGE(D5,D8)</f>
         <v>0.62</v>
       </c>
-      <c r="E14" s="27">
+      <c r="E14" s="26">
         <f>AVERAGE(E2,E8)</f>
         <v>1.9</v>
       </c>
@@ -4404,7 +4403,7 @@
         <v>59.400998287645102</v>
       </c>
     </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A15" s="1">
         <v>2</v>
       </c>
@@ -4419,7 +4418,7 @@
         <f t="shared" ref="D15:D16" si="0">AVERAGE(D6,D9)</f>
         <v>0.71500000000000008</v>
       </c>
-      <c r="E15" s="27">
+      <c r="E15" s="26">
         <f t="shared" ref="E15:E16" si="1">AVERAGE(E3,E9)</f>
         <v>2.27</v>
       </c>
@@ -4427,7 +4426,7 @@
         <v>60.554081661965597</v>
       </c>
     </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A16" s="1">
         <v>3</v>
       </c>
@@ -4442,7 +4441,7 @@
         <f t="shared" si="0"/>
         <v>0.495</v>
       </c>
-      <c r="E16" s="27">
+      <c r="E16" s="26">
         <f t="shared" si="1"/>
         <v>1.1850000000000001</v>
       </c>
@@ -4450,10 +4449,10 @@
         <v>51.300016366594399</v>
       </c>
     </row>
-    <row r="17" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D17" s="4"/>
     </row>
-    <row r="18" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D18" s="4"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added csf-con and csf-rrm plots
</commit_message>
<xml_diff>
--- a/out.xlsx
+++ b/out.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\uphjan2\Projects\screen-audit\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76606C53-6FA7-40C0-B3F8-FE269344121C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8D8041E-B530-435B-BD3F-4B131BC6C63D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-24120" yWindow="-120" windowWidth="24240" windowHeight="13140" tabRatio="500" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-24120" yWindow="-120" windowWidth="24240" windowHeight="13140" tabRatio="500" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="out" sheetId="1" r:id="rId1"/>
@@ -20,6 +20,7 @@
     <sheet name="FAR-rrm" sheetId="4" r:id="rId5"/>
     <sheet name="FAR-csf" sheetId="5" r:id="rId6"/>
     <sheet name="FAR-con" sheetId="6" r:id="rId7"/>
+    <sheet name="FPI" sheetId="8" r:id="rId8"/>
   </sheets>
   <calcPr calcId="191029" iterateDelta="1E-4"/>
   <extLst>
@@ -39,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="261" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="262" uniqueCount="94">
   <si>
     <t>trial</t>
   </si>
@@ -302,9 +303,6 @@
     <t>SD</t>
   </si>
   <si>
-    <t>Rrmt</t>
-  </si>
-  <si>
     <t>Combined</t>
   </si>
   <si>
@@ -321,6 +319,9 @@
   </si>
   <si>
     <t>%</t>
+  </si>
+  <si>
+    <t>CSFdrop</t>
   </si>
 </sst>
 </file>
@@ -425,7 +426,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -479,9 +480,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
@@ -894,7 +892,7 @@
   <dimension ref="A1:AMJ26"/>
   <sheetViews>
     <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1779,19 +1777,19 @@
       </c>
     </row>
     <row r="24" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="J24" s="20">
+      <c r="J24" s="19">
         <f>J2*3</f>
         <v>996.9782399999998</v>
       </c>
     </row>
     <row r="25" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="J25" s="20">
+      <c r="J25" s="19">
         <f>J9*3</f>
         <v>972.85536000000002</v>
       </c>
     </row>
     <row r="26" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="J26" s="20">
+      <c r="J26" s="19">
         <f>J16*3</f>
         <v>856.45728000000008</v>
       </c>
@@ -1822,36 +1820,36 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B2" s="21"/>
-      <c r="C2" s="21" t="s">
+      <c r="B2" s="20"/>
+      <c r="C2" s="20" t="s">
+        <v>88</v>
+      </c>
+      <c r="D2" s="24" t="s">
         <v>89</v>
       </c>
-      <c r="D2" s="25" t="s">
+      <c r="E2" s="26" t="s">
         <v>90</v>
       </c>
-      <c r="E2" s="27" t="s">
+      <c r="F2" s="26"/>
+      <c r="G2" s="26"/>
+    </row>
+    <row r="3" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B3" s="21" t="s">
+        <v>66</v>
+      </c>
+      <c r="C3" s="21" t="s">
         <v>91</v>
       </c>
-      <c r="F2" s="27"/>
-      <c r="G2" s="27"/>
-    </row>
-    <row r="3" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B3" s="22" t="s">
-        <v>66</v>
-      </c>
-      <c r="C3" s="22" t="s">
+      <c r="D3" s="21" t="s">
         <v>92</v>
       </c>
-      <c r="D3" s="22" t="s">
-        <v>93</v>
-      </c>
-      <c r="E3" s="22" t="s">
+      <c r="E3" s="21" t="s">
         <v>80</v>
       </c>
-      <c r="F3" s="22" t="s">
+      <c r="F3" s="21" t="s">
         <v>81</v>
       </c>
-      <c r="G3" s="22" t="s">
+      <c r="G3" s="21" t="s">
         <v>82</v>
       </c>
     </row>
@@ -1859,19 +1857,19 @@
       <c r="B4" s="1">
         <v>1</v>
       </c>
-      <c r="C4" s="20">
+      <c r="C4" s="19">
         <v>996.9782399999998</v>
       </c>
-      <c r="D4" s="24">
+      <c r="D4" s="23">
         <v>1.3</v>
       </c>
-      <c r="E4" s="23">
+      <c r="E4" s="22">
         <v>25</v>
       </c>
-      <c r="F4" s="23">
+      <c r="F4" s="22">
         <v>22</v>
       </c>
-      <c r="G4" s="23">
+      <c r="G4" s="22">
         <v>42</v>
       </c>
     </row>
@@ -1879,19 +1877,19 @@
       <c r="B5" s="1">
         <v>2</v>
       </c>
-      <c r="C5" s="20">
+      <c r="C5" s="19">
         <v>972.85536000000002</v>
       </c>
-      <c r="D5" s="24">
+      <c r="D5" s="23">
         <v>1.55</v>
       </c>
-      <c r="E5" s="23">
+      <c r="E5" s="22">
         <v>25</v>
       </c>
-      <c r="F5" s="23">
+      <c r="F5" s="22">
         <v>22</v>
       </c>
-      <c r="G5" s="23">
+      <c r="G5" s="22">
         <v>42</v>
       </c>
     </row>
@@ -1899,19 +1897,19 @@
       <c r="B6" s="1">
         <v>3</v>
       </c>
-      <c r="C6" s="20">
+      <c r="C6" s="19">
         <v>856.45728000000008</v>
       </c>
-      <c r="D6" s="24">
+      <c r="D6" s="23">
         <v>1</v>
       </c>
-      <c r="E6" s="23">
+      <c r="E6" s="22">
         <v>25</v>
       </c>
-      <c r="F6" s="23">
+      <c r="F6" s="22">
         <v>22</v>
       </c>
-      <c r="G6" s="23">
+      <c r="G6" s="22">
         <v>38</v>
       </c>
     </row>
@@ -3569,8 +3567,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:AMJ18"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J23" sqref="J23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3582,7 +3580,7 @@
     <col min="8" max="1024" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>66</v>
       </c>
@@ -3604,8 +3602,11 @@
       <c r="G1" s="2" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H1" s="21" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -3630,8 +3631,12 @@
       <c r="G2" s="4">
         <v>41.438818163172797</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H2" s="19">
+        <f t="shared" ref="H2:H13" si="0">C2-D2</f>
+        <v>41</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -3656,8 +3661,12 @@
       <c r="G3" s="4">
         <v>40.319629836854702</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H3" s="19">
+        <f t="shared" si="0"/>
+        <v>91</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -3682,8 +3691,12 @@
       <c r="G4" s="4">
         <v>35.632516311846899</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H4" s="19">
+        <f t="shared" si="0"/>
+        <v>71</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
         <v>1</v>
       </c>
@@ -3708,8 +3721,12 @@
       <c r="G5" s="4">
         <v>43.686509816306099</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H5" s="19">
+        <f t="shared" si="0"/>
+        <v>82</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
         <v>2</v>
       </c>
@@ -3734,8 +3751,12 @@
       <c r="G6" s="4">
         <v>47.032349220362001</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H6" s="19">
+        <f t="shared" si="0"/>
+        <v>62</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
         <v>3</v>
       </c>
@@ -3760,8 +3781,12 @@
       <c r="G7" s="4">
         <v>41.477432015699499</v>
       </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H7" s="19">
+        <f t="shared" si="0"/>
+        <v>46</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
         <v>1</v>
       </c>
@@ -3786,8 +3811,12 @@
       <c r="G8" s="4">
         <v>70.210467498603094</v>
       </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H8" s="19">
+        <f t="shared" si="0"/>
+        <v>109</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
         <v>2</v>
       </c>
@@ -3812,8 +3841,12 @@
       <c r="G9" s="4">
         <v>72.088047577603703</v>
       </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H9" s="19">
+        <f t="shared" si="0"/>
+        <v>176</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
         <v>3</v>
       </c>
@@ -3838,8 +3871,12 @@
       <c r="G10" s="4">
         <v>58.684216832822102</v>
       </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H10" s="19">
+        <f t="shared" si="0"/>
+        <v>118</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>86</v>
       </c>
@@ -3866,8 +3903,12 @@
         <f>_xlfn.STDEV.P(G2:G4)</f>
         <v>2.5151707893144999</v>
       </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H11" s="19">
+        <f t="shared" si="0"/>
+        <v>18.19732762431795</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>86</v>
       </c>
@@ -3894,8 +3935,12 @@
         <f>_xlfn.STDEV.P(G5:G7)</f>
         <v>2.2835588987738102</v>
       </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H12" s="19">
+        <f t="shared" si="0"/>
+        <v>-10.293878958713464</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>86</v>
       </c>
@@ -3922,13 +3967,17 @@
         <f>_xlfn.STDEV.P(G8:G10)</f>
         <v>5.9258608375889077</v>
       </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H13" s="19">
+        <f t="shared" si="0"/>
+        <v>18.907097433455025</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A14" s="1">
         <v>1</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C14" s="1">
         <f>C2</f>
@@ -3948,24 +3997,28 @@
       <c r="G14" s="4">
         <v>59.400998287645145</v>
       </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H14" s="19">
+        <f>C14-D14</f>
+        <v>117</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A15" s="1">
         <v>2</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C15" s="1">
-        <f t="shared" ref="C15:C16" si="0">C3</f>
+        <f t="shared" ref="C15:C16" si="1">C3</f>
         <v>191</v>
       </c>
       <c r="D15" s="4">
-        <f t="shared" ref="D15:D16" si="1">AVERAGE(D6,D9)</f>
+        <f t="shared" ref="D15:D16" si="2">AVERAGE(D6,D9)</f>
         <v>38</v>
       </c>
       <c r="E15" s="1">
-        <f t="shared" ref="E15:E16" si="2">AVERAGE(E3,E9)</f>
+        <f t="shared" ref="E15:E16" si="3">AVERAGE(E3,E9)</f>
         <v>377.5</v>
       </c>
       <c r="F15" s="4">
@@ -3974,24 +4027,28 @@
       <c r="G15" s="4">
         <v>60.554081661965562</v>
       </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H15" s="19">
+        <f t="shared" ref="H15:H16" si="4">C15-D15</f>
+        <v>153</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A16" s="1">
         <v>3</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C16" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>165</v>
       </c>
       <c r="D16" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>53</v>
       </c>
       <c r="E16" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>338.5</v>
       </c>
       <c r="F16" s="4">
@@ -4000,6 +4057,10 @@
       <c r="G16" s="4">
         <v>51.300016366594406</v>
       </c>
+      <c r="H16" s="19">
+        <f t="shared" si="4"/>
+        <v>112</v>
+      </c>
     </row>
     <row r="17" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D17" s="4"/>
@@ -4009,7 +4070,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -4017,8 +4078,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:AMJ18"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G21" sqref="G21"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H26" sqref="H26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4052,8 +4113,8 @@
       <c r="G1" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="H1" s="19" t="s">
-        <v>87</v>
+      <c r="H1" s="21" t="s">
+        <v>93</v>
       </c>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.3">
@@ -4081,7 +4142,9 @@
       <c r="G2" s="4">
         <v>41.438818163172797</v>
       </c>
-      <c r="H2"/>
+      <c r="H2" s="19">
+        <v>41</v>
+      </c>
       <c r="R2" s="4"/>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.3">
@@ -4109,7 +4172,9 @@
       <c r="G3" s="4">
         <v>40.319629836854702</v>
       </c>
-      <c r="H3"/>
+      <c r="H3" s="19">
+        <v>91</v>
+      </c>
       <c r="R3" s="4"/>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.3">
@@ -4137,7 +4202,9 @@
       <c r="G4" s="4">
         <v>35.632516311846899</v>
       </c>
-      <c r="H4"/>
+      <c r="H4" s="19">
+        <v>71</v>
+      </c>
       <c r="R4" s="4"/>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.3">
@@ -4165,6 +4232,9 @@
       <c r="G5" s="4">
         <v>43.686509816306099</v>
       </c>
+      <c r="H5" s="19">
+        <v>82</v>
+      </c>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
@@ -4191,6 +4261,9 @@
       <c r="G6" s="4">
         <v>47.032349220362001</v>
       </c>
+      <c r="H6" s="19">
+        <v>62</v>
+      </c>
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
@@ -4217,6 +4290,9 @@
       <c r="G7" s="4">
         <v>41.477432015699499</v>
       </c>
+      <c r="H7" s="19">
+        <v>46</v>
+      </c>
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
@@ -4243,6 +4319,9 @@
       <c r="G8" s="4">
         <v>70.210467498603094</v>
       </c>
+      <c r="H8" s="19">
+        <v>109</v>
+      </c>
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
@@ -4269,6 +4348,9 @@
       <c r="G9" s="4">
         <v>72.088047577603703</v>
       </c>
+      <c r="H9" s="19">
+        <v>176</v>
+      </c>
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
@@ -4295,6 +4377,9 @@
       <c r="G10" s="4">
         <v>58.684216832822102</v>
       </c>
+      <c r="H10" s="19">
+        <v>118</v>
+      </c>
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
@@ -4323,6 +4408,9 @@
         <f>_xlfn.STDEV.P(G2:G4)</f>
         <v>2.5151707893144999</v>
       </c>
+      <c r="H11" s="19">
+        <v>18.19732762431795</v>
+      </c>
     </row>
     <row r="12" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
@@ -4351,6 +4439,9 @@
         <f>_xlfn.STDEV.P(G5:G7)</f>
         <v>2.2835588987738102</v>
       </c>
+      <c r="H12" s="19">
+        <v>-10.293878958713464</v>
+      </c>
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
@@ -4379,13 +4470,16 @@
         <f>_xlfn.STDEV.P(G8:G10)</f>
         <v>5.9258608375889077</v>
       </c>
+      <c r="H13" s="19">
+        <v>18.907097433455025</v>
+      </c>
     </row>
     <row r="14" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A14" s="1">
         <v>1</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C14" s="1">
         <f>C2</f>
@@ -4395,12 +4489,15 @@
         <f>AVERAGE(D5,D8)</f>
         <v>0.62</v>
       </c>
-      <c r="E14" s="26">
+      <c r="E14" s="25">
         <f>AVERAGE(E2,E8)</f>
         <v>1.9</v>
       </c>
       <c r="G14" s="4">
         <v>59.400998287645102</v>
+      </c>
+      <c r="H14" s="19">
+        <v>117</v>
       </c>
     </row>
     <row r="15" spans="1:18" x14ac:dyDescent="0.3">
@@ -4408,7 +4505,7 @@
         <v>2</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C15" s="1">
         <f>C3</f>
@@ -4418,12 +4515,15 @@
         <f t="shared" ref="D15:D16" si="0">AVERAGE(D6,D9)</f>
         <v>0.71500000000000008</v>
       </c>
-      <c r="E15" s="26">
+      <c r="E15" s="25">
         <f t="shared" ref="E15:E16" si="1">AVERAGE(E3,E9)</f>
         <v>2.27</v>
       </c>
       <c r="G15" s="4">
         <v>60.554081661965597</v>
+      </c>
+      <c r="H15" s="19">
+        <v>153</v>
       </c>
     </row>
     <row r="16" spans="1:18" x14ac:dyDescent="0.3">
@@ -4431,7 +4531,7 @@
         <v>3</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C16" s="1">
         <f>C4</f>
@@ -4441,12 +4541,15 @@
         <f t="shared" si="0"/>
         <v>0.495</v>
       </c>
-      <c r="E16" s="26">
+      <c r="E16" s="25">
         <f t="shared" si="1"/>
         <v>1.1850000000000001</v>
       </c>
       <c r="G16" s="4">
         <v>51.300016366594399</v>
+      </c>
+      <c r="H16" s="19">
+        <v>112</v>
       </c>
     </row>
     <row r="17" spans="4:4" x14ac:dyDescent="0.3">
@@ -4459,4 +4562,18 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{69F48122-4A28-482A-9135-507475642A28}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="O9" sqref="O9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
added new samples to out.xlsx
</commit_message>
<xml_diff>
--- a/out.xlsx
+++ b/out.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\uphjan2\Projects\screen-audit\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8D8041E-B530-435B-BD3F-4B131BC6C63D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9C50109-7405-416F-B382-3F677097DB19}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-24120" yWindow="-120" windowWidth="24240" windowHeight="13140" tabRatio="500" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-24120" yWindow="-120" windowWidth="24240" windowHeight="13140" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="out" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
     <sheet name="FAR-con" sheetId="6" r:id="rId7"/>
     <sheet name="FPI" sheetId="8" r:id="rId8"/>
   </sheets>
-  <calcPr calcId="191029" iterateDelta="1E-4"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="262" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="304" uniqueCount="94">
   <si>
     <t>trial</t>
   </si>
@@ -328,11 +328,12 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="0.0"/>
     <numFmt numFmtId="165" formatCode="0.0%"/>
+    <numFmt numFmtId="166" formatCode="0.000"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -360,6 +361,11 @@
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -426,7 +432,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -505,6 +511,21 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -889,10 +910,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AMJ26"/>
+  <dimension ref="A1:AMJ36"/>
   <sheetViews>
-    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="K31" sqref="K31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1736,62 +1757,436 @@
       <c r="K21" s="4"/>
     </row>
     <row r="22" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A22" s="1">
+      <c r="A22" s="9">
         <v>20</v>
       </c>
-      <c r="B22" s="1">
+      <c r="B22" s="9">
         <v>3</v>
       </c>
-      <c r="C22" s="1" t="s">
+      <c r="C22" s="9" t="s">
         <v>42</v>
       </c>
-      <c r="D22" s="1" t="s">
+      <c r="D22" s="9" t="s">
         <v>59</v>
       </c>
-      <c r="E22" s="1">
+      <c r="E22" s="9">
         <v>0.98</v>
       </c>
-      <c r="F22" s="7">
+      <c r="F22" s="10">
         <v>332</v>
       </c>
-      <c r="G22" s="1">
+      <c r="G22" s="9">
         <v>3998</v>
       </c>
-      <c r="H22" s="1" t="s">
+      <c r="H22" s="9" t="s">
         <v>44</v>
       </c>
-      <c r="I22" s="1" t="s">
+      <c r="I22" s="9" t="s">
         <v>45</v>
       </c>
-      <c r="J22" s="4">
+      <c r="J22" s="11">
         <v>62.688639999999999</v>
       </c>
-      <c r="K22" s="4"/>
-      <c r="O22" s="5">
+      <c r="K22" s="11"/>
+      <c r="L22" s="9"/>
+      <c r="M22" s="9"/>
+      <c r="N22" s="9"/>
+      <c r="O22" s="12">
         <f>G22/G20</f>
         <v>0.38324386503067487</v>
       </c>
-      <c r="P22" s="5">
+      <c r="P22" s="12">
         <f>J22/J20</f>
         <v>0.58684216832822089</v>
       </c>
     </row>
+    <row r="23" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A23" s="1">
+        <v>21</v>
+      </c>
+      <c r="B23" s="1">
+        <v>4</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D23" s="1" t="str">
+        <f>_xlfn.CONCAT(C23,B23)</f>
+        <v>A4</v>
+      </c>
+      <c r="E23" s="27">
+        <v>1.24</v>
+      </c>
+      <c r="F23" s="28">
+        <v>196</v>
+      </c>
+      <c r="H23" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="I23" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
     <row r="24" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="J24" s="19">
-        <f>J2*3</f>
-        <v>996.9782399999998</v>
-      </c>
+      <c r="A24" s="1">
+        <v>22</v>
+      </c>
+      <c r="B24" s="1">
+        <v>4</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D24" s="1" t="str">
+        <f t="shared" ref="D24:D36" si="0">_xlfn.CONCAT(C24,B24)</f>
+        <v>B4</v>
+      </c>
+      <c r="E24" s="27">
+        <v>2.04</v>
+      </c>
+      <c r="F24" s="28">
+        <v>347</v>
+      </c>
+      <c r="H24" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="I24" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="J24" s="19"/>
     </row>
     <row r="25" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="J25" s="19">
-        <f>J9*3</f>
-        <v>972.85536000000002</v>
-      </c>
+      <c r="A25" s="1">
+        <v>23</v>
+      </c>
+      <c r="B25" s="1">
+        <v>4</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D25" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>C4</v>
+      </c>
+      <c r="E25" s="27">
+        <v>1.01</v>
+      </c>
+      <c r="F25" s="28">
+        <v>90</v>
+      </c>
+      <c r="H25" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="I25" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="J25" s="19"/>
     </row>
     <row r="26" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="J26" s="19">
-        <f>J16*3</f>
-        <v>856.45728000000008</v>
+      <c r="A26" s="1">
+        <v>24</v>
+      </c>
+      <c r="B26" s="1">
+        <v>4</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D26" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>D4</v>
+      </c>
+      <c r="E26" s="29">
+        <v>0.71899999999999997</v>
+      </c>
+      <c r="F26" s="28">
+        <v>41</v>
+      </c>
+      <c r="H26" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="I26" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="J26" s="19"/>
+    </row>
+    <row r="27" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A27" s="1">
+        <v>25</v>
+      </c>
+      <c r="B27" s="1">
+        <v>4</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D27" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>E4</v>
+      </c>
+      <c r="E27" s="29">
+        <v>0.82399999999999995</v>
+      </c>
+      <c r="F27" s="28">
+        <v>184</v>
+      </c>
+      <c r="H27" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="I27" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="28" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A28" s="1">
+        <v>26</v>
+      </c>
+      <c r="B28" s="1">
+        <v>4</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D28" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>F4</v>
+      </c>
+      <c r="E28" s="29">
+        <v>0.44500000000000001</v>
+      </c>
+      <c r="F28" s="28">
+        <v>46</v>
+      </c>
+      <c r="H28" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="I28" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="29" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A29" s="9">
+        <v>27</v>
+      </c>
+      <c r="B29" s="9">
+        <v>4</v>
+      </c>
+      <c r="C29" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="D29" s="9" t="str">
+        <f t="shared" si="0"/>
+        <v>G4</v>
+      </c>
+      <c r="E29" s="30">
+        <v>1.36</v>
+      </c>
+      <c r="F29" s="31">
+        <v>320</v>
+      </c>
+      <c r="G29" s="9"/>
+      <c r="H29" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="I29" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="J29" s="9"/>
+      <c r="K29" s="9"/>
+      <c r="L29" s="9"/>
+      <c r="M29" s="9"/>
+      <c r="N29" s="9"/>
+      <c r="O29" s="9"/>
+      <c r="P29" s="9"/>
+    </row>
+    <row r="30" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A30" s="1">
+        <v>28</v>
+      </c>
+      <c r="B30" s="1">
+        <v>5</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D30" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>A5</v>
+      </c>
+      <c r="E30" s="27">
+        <v>1.04</v>
+      </c>
+      <c r="F30" s="28">
+        <v>166</v>
+      </c>
+      <c r="H30" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="I30" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="31" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A31" s="1">
+        <v>29</v>
+      </c>
+      <c r="B31" s="1">
+        <v>5</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D31" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>B5</v>
+      </c>
+      <c r="E31" s="27">
+        <v>1.76</v>
+      </c>
+      <c r="F31" s="28">
+        <v>359</v>
+      </c>
+      <c r="H31" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="I31" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="32" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A32" s="1">
+        <v>30</v>
+      </c>
+      <c r="B32" s="1">
+        <v>5</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D32" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>C5</v>
+      </c>
+      <c r="E32" s="29">
+        <v>0.91800000000000004</v>
+      </c>
+      <c r="F32" s="28">
+        <v>95</v>
+      </c>
+      <c r="H32" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="I32" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A33" s="1">
+        <v>31</v>
+      </c>
+      <c r="B33" s="1">
+        <v>5</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D33" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>D5</v>
+      </c>
+      <c r="E33" s="29">
+        <v>0.71499999999999997</v>
+      </c>
+      <c r="F33" s="28">
+        <v>48</v>
+      </c>
+      <c r="H33" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="I33" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A34" s="1">
+        <v>32</v>
+      </c>
+      <c r="B34" s="1">
+        <v>5</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D34" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>E5</v>
+      </c>
+      <c r="E34" s="29">
+        <v>0.79300000000000004</v>
+      </c>
+      <c r="F34" s="28">
+        <v>190</v>
+      </c>
+      <c r="H34" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="I34" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A35" s="1">
+        <v>33</v>
+      </c>
+      <c r="B35" s="1">
+        <v>5</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D35" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>F5</v>
+      </c>
+      <c r="E35" s="29">
+        <v>0.44700000000000001</v>
+      </c>
+      <c r="F35" s="28">
+        <v>52</v>
+      </c>
+      <c r="H35" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="I35" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A36" s="1">
+        <v>34</v>
+      </c>
+      <c r="B36" s="1">
+        <v>5</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D36" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>G5</v>
+      </c>
+      <c r="E36" s="27">
+        <v>1.27</v>
+      </c>
+      <c r="F36" s="28">
+        <v>330</v>
+      </c>
+      <c r="H36" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="I36" s="9" t="s">
+        <v>45</v>
       </c>
     </row>
   </sheetData>
@@ -3567,7 +3962,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:AMJ18"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="J23" sqref="J23"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
added trials 4 and 5
</commit_message>
<xml_diff>
--- a/out.xlsx
+++ b/out.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\uphjan2\Projects\screen-audit\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9C50109-7405-416F-B382-3F677097DB19}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6CE120A-97A2-4197-90D6-4E5656F072B8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-24120" yWindow="-120" windowWidth="24240" windowHeight="13140" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-24120" yWindow="-120" windowWidth="24240" windowHeight="13140" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="out" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,8 @@
     <sheet name="FAR-rrm" sheetId="4" r:id="rId5"/>
     <sheet name="FAR-csf" sheetId="5" r:id="rId6"/>
     <sheet name="FAR-con" sheetId="6" r:id="rId7"/>
-    <sheet name="FPI" sheetId="8" r:id="rId8"/>
+    <sheet name="FAR-con2" sheetId="9" r:id="rId8"/>
+    <sheet name="FPI" sheetId="8" r:id="rId9"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -40,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="304" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="394" uniqueCount="96">
   <si>
     <t>trial</t>
   </si>
@@ -322,6 +323,12 @@
   </si>
   <si>
     <t>CSFdrop</t>
+  </si>
+  <si>
+    <t>Screen2</t>
+  </si>
+  <si>
+    <t>Date</t>
   </si>
 </sst>
 </file>
@@ -432,7 +439,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -509,9 +516,6 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="2" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -526,6 +530,38 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="2" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -912,8 +948,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AMJ36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="K31" sqref="K31"/>
+    <sheetView topLeftCell="C1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection activeCell="C1" sqref="C1"/>
+      <selection pane="bottomLeft" activeCell="K1" sqref="K1:T1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1061,6 +1099,7 @@
         <v>25</v>
       </c>
       <c r="J3" s="4">
+        <f>E3*G3/62.5</f>
         <v>137.71199999999999</v>
       </c>
       <c r="K3" s="5">
@@ -1102,6 +1141,7 @@
         <v>29</v>
       </c>
       <c r="J4" s="4">
+        <f t="shared" ref="J4:J8" si="0">E4*G4/62.5</f>
         <v>145.91231999999999</v>
       </c>
       <c r="K4" s="4"/>
@@ -1135,7 +1175,8 @@
         <v>33</v>
       </c>
       <c r="J5" s="4">
-        <v>82.168319999999994</v>
+        <f t="shared" si="0"/>
+        <v>82.168320000000008</v>
       </c>
       <c r="K5" s="4"/>
       <c r="M5" s="5">
@@ -1144,7 +1185,7 @@
       </c>
       <c r="N5" s="5">
         <f>(J4-J5)/J4</f>
-        <v>0.43686509816306124</v>
+        <v>0.43686509816306113</v>
       </c>
       <c r="O5" s="5"/>
     </row>
@@ -1177,6 +1218,7 @@
         <v>37</v>
       </c>
       <c r="J6" s="4">
+        <f t="shared" si="0"/>
         <v>120.26560000000001</v>
       </c>
       <c r="K6" s="4"/>
@@ -1210,7 +1252,8 @@
         <v>41</v>
       </c>
       <c r="J7" s="4">
-        <v>35.077759999999998</v>
+        <f t="shared" si="0"/>
+        <v>35.077760000000005</v>
       </c>
       <c r="K7" s="4"/>
     </row>
@@ -1243,6 +1286,7 @@
         <v>45</v>
       </c>
       <c r="J8" s="11">
+        <f t="shared" si="0"/>
         <v>84.439040000000006</v>
       </c>
       <c r="K8" s="11"/>
@@ -1574,7 +1618,7 @@
         <v>0.50271574549521014</v>
       </c>
     </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A17" s="1">
         <v>15</v>
       </c>
@@ -1615,7 +1659,7 @@
       </c>
       <c r="M17" s="5"/>
     </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A18" s="1">
         <v>16</v>
       </c>
@@ -1648,7 +1692,7 @@
       </c>
       <c r="K18" s="4"/>
     </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A19" s="1">
         <v>17</v>
       </c>
@@ -1690,7 +1734,7 @@
       </c>
       <c r="O19" s="5"/>
     </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A20" s="1">
         <v>18</v>
       </c>
@@ -1723,7 +1767,7 @@
       </c>
       <c r="K20" s="4"/>
     </row>
-    <row r="21" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A21" s="1">
         <v>19</v>
       </c>
@@ -1756,7 +1800,7 @@
       </c>
       <c r="K21" s="4"/>
     </row>
-    <row r="22" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A22" s="9">
         <v>20</v>
       </c>
@@ -1800,7 +1844,7 @@
         <v>0.58684216832822089</v>
       </c>
     </row>
-    <row r="23" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A23" s="1">
         <v>21</v>
       </c>
@@ -1814,11 +1858,14 @@
         <f>_xlfn.CONCAT(C23,B23)</f>
         <v>A4</v>
       </c>
-      <c r="E23" s="27">
+      <c r="E23" s="26">
         <v>1.24</v>
       </c>
-      <c r="F23" s="28">
+      <c r="F23" s="27">
         <v>196</v>
+      </c>
+      <c r="G23" s="1">
+        <v>16476.587011718751</v>
       </c>
       <c r="H23" s="1" t="s">
         <v>20</v>
@@ -1826,8 +1873,25 @@
       <c r="I23" s="1" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="24" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="J23" s="4">
+        <f>E23*G23/62.5</f>
+        <v>326.89548631250005</v>
+      </c>
+      <c r="K23" s="4"/>
+      <c r="R23" s="4">
+        <f>J23*3</f>
+        <v>980.68645893750022</v>
+      </c>
+      <c r="S23" s="4">
+        <f>J24*3 + J29*2</f>
+        <v>536.47147456250002</v>
+      </c>
+      <c r="T23" s="5">
+        <f>S23/R23</f>
+        <v>0.54703669014021705</v>
+      </c>
+    </row>
+    <row r="24" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A24" s="1">
         <v>22</v>
       </c>
@@ -1838,14 +1902,17 @@
         <v>22</v>
       </c>
       <c r="D24" s="1" t="str">
-        <f t="shared" ref="D24:D36" si="0">_xlfn.CONCAT(C24,B24)</f>
+        <f t="shared" ref="D24:D36" si="1">_xlfn.CONCAT(C24,B24)</f>
         <v>B4</v>
       </c>
-      <c r="E24" s="27">
+      <c r="E24" s="26">
         <v>2.04</v>
       </c>
-      <c r="F24" s="28">
+      <c r="F24" s="27">
         <v>347</v>
+      </c>
+      <c r="G24" s="1">
+        <v>3958.6252929687498</v>
       </c>
       <c r="H24" s="1" t="s">
         <v>24</v>
@@ -1853,9 +1920,21 @@
       <c r="I24" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="J24" s="19"/>
-    </row>
-    <row r="25" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="J24" s="4">
+        <f>E24*G24/62.5</f>
+        <v>129.20952956249999</v>
+      </c>
+      <c r="K24" s="5">
+        <f>G24/G23</f>
+        <v>0.240257602509138</v>
+      </c>
+      <c r="L24" s="5">
+        <f>J24/J23</f>
+        <v>0.39526250735374313</v>
+      </c>
+      <c r="M24" s="5"/>
+    </row>
+    <row r="25" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A25" s="1">
         <v>23</v>
       </c>
@@ -1866,14 +1945,17 @@
         <v>26</v>
       </c>
       <c r="D25" s="1" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>C4</v>
       </c>
-      <c r="E25" s="27">
+      <c r="E25" s="26">
         <v>1.01</v>
       </c>
-      <c r="F25" s="28">
+      <c r="F25" s="27">
         <v>90</v>
+      </c>
+      <c r="G25" s="1">
+        <v>9649.0945556640636</v>
       </c>
       <c r="H25" s="1" t="s">
         <v>28</v>
@@ -1881,9 +1963,13 @@
       <c r="I25" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="J25" s="19"/>
-    </row>
-    <row r="26" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="J25" s="4">
+        <f t="shared" ref="J25:J29" si="2">E25*G25/62.5</f>
+        <v>155.92936801953127</v>
+      </c>
+      <c r="K25" s="4"/>
+    </row>
+    <row r="26" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A26" s="1">
         <v>24</v>
       </c>
@@ -1894,14 +1980,17 @@
         <v>30</v>
       </c>
       <c r="D26" s="1" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>D4</v>
       </c>
-      <c r="E26" s="29">
+      <c r="E26" s="28">
         <v>0.71899999999999997</v>
       </c>
-      <c r="F26" s="28">
+      <c r="F26" s="27">
         <v>41</v>
+      </c>
+      <c r="G26" s="1">
+        <v>7715.1844726562504</v>
       </c>
       <c r="H26" s="1" t="s">
         <v>32</v>
@@ -1909,9 +1998,22 @@
       <c r="I26" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="J26" s="19"/>
-    </row>
-    <row r="27" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="J26" s="4">
+        <f t="shared" si="2"/>
+        <v>88.7554821734375</v>
+      </c>
+      <c r="K26" s="4"/>
+      <c r="M26" s="5">
+        <f>(G25-G26)/G25</f>
+        <v>0.20042399541753883</v>
+      </c>
+      <c r="N26" s="5">
+        <f>(J25-J26)/J25</f>
+        <v>0.43079688386654502</v>
+      </c>
+      <c r="O26" s="5"/>
+    </row>
+    <row r="27" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A27" s="1">
         <v>25</v>
       </c>
@@ -1922,14 +2024,17 @@
         <v>34</v>
       </c>
       <c r="D27" s="1" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>E4</v>
       </c>
-      <c r="E27" s="29">
+      <c r="E27" s="28">
         <v>0.82399999999999995</v>
       </c>
-      <c r="F27" s="28">
+      <c r="F27" s="27">
         <v>184</v>
+      </c>
+      <c r="G27" s="1">
+        <v>8525.7999999999993</v>
       </c>
       <c r="H27" s="1" t="s">
         <v>36</v>
@@ -1937,8 +2042,13 @@
       <c r="I27" s="1" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="28" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="J27" s="4">
+        <f t="shared" si="2"/>
+        <v>112.40414719999998</v>
+      </c>
+      <c r="K27" s="4"/>
+    </row>
+    <row r="28" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A28" s="1">
         <v>26</v>
       </c>
@@ -1949,14 +2059,17 @@
         <v>38</v>
       </c>
       <c r="D28" s="1" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>F4</v>
       </c>
-      <c r="E28" s="29">
+      <c r="E28" s="28">
         <v>0.44500000000000001</v>
       </c>
-      <c r="F28" s="28">
+      <c r="F28" s="27">
         <v>46</v>
+      </c>
+      <c r="G28" s="1">
+        <v>5119.9598632812504</v>
       </c>
       <c r="H28" s="1" t="s">
         <v>40</v>
@@ -1964,8 +2077,13 @@
       <c r="I28" s="1" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="29" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="J28" s="4">
+        <f t="shared" si="2"/>
+        <v>36.454114226562503</v>
+      </c>
+      <c r="K28" s="4"/>
+    </row>
+    <row r="29" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A29" s="9">
         <v>27</v>
       </c>
@@ -1976,31 +2094,42 @@
         <v>42</v>
       </c>
       <c r="D29" s="9" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>G4</v>
       </c>
-      <c r="E29" s="30">
+      <c r="E29" s="29">
         <v>1.36</v>
       </c>
-      <c r="F29" s="31">
+      <c r="F29" s="30">
         <v>320</v>
       </c>
-      <c r="G29" s="9"/>
+      <c r="G29" s="9">
+        <v>3420.1030761718748</v>
+      </c>
       <c r="H29" s="9" t="s">
         <v>44</v>
       </c>
       <c r="I29" s="9" t="s">
         <v>45</v>
       </c>
-      <c r="J29" s="9"/>
-      <c r="K29" s="9"/>
+      <c r="J29" s="11">
+        <f t="shared" si="2"/>
+        <v>74.421442937500004</v>
+      </c>
+      <c r="K29" s="11"/>
       <c r="L29" s="9"/>
       <c r="M29" s="9"/>
       <c r="N29" s="9"/>
-      <c r="O29" s="9"/>
-      <c r="P29" s="9"/>
-    </row>
-    <row r="30" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="O29" s="12">
+        <f>G29/G27</f>
+        <v>0.40114746723731204</v>
+      </c>
+      <c r="P29" s="12">
+        <f>J29/J27</f>
+        <v>0.66208805272177729</v>
+      </c>
+    </row>
+    <row r="30" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A30" s="1">
         <v>28</v>
       </c>
@@ -2011,14 +2140,17 @@
         <v>18</v>
       </c>
       <c r="D30" s="1" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>A5</v>
       </c>
-      <c r="E30" s="27">
+      <c r="E30" s="26">
         <v>1.04</v>
       </c>
-      <c r="F30" s="28">
+      <c r="F30" s="27">
         <v>166</v>
+      </c>
+      <c r="G30" s="36">
+        <v>17108.699121093749</v>
       </c>
       <c r="H30" s="1" t="s">
         <v>20</v>
@@ -2026,8 +2158,25 @@
       <c r="I30" s="1" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="31" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="J30" s="4">
+        <f>E30*G30/62.5</f>
+        <v>284.68875337499998</v>
+      </c>
+      <c r="K30" s="4"/>
+      <c r="R30" s="4">
+        <f>J30*3</f>
+        <v>854.06626012499987</v>
+      </c>
+      <c r="S30" s="4">
+        <f>J31*3 + J36*2</f>
+        <v>480.74249803124997</v>
+      </c>
+      <c r="T30" s="5">
+        <f>S30/R30</f>
+        <v>0.56288665233173973</v>
+      </c>
+    </row>
+    <row r="31" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A31" s="1">
         <v>29</v>
       </c>
@@ -2038,14 +2187,17 @@
         <v>22</v>
       </c>
       <c r="D31" s="1" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>B5</v>
       </c>
-      <c r="E31" s="27">
+      <c r="E31" s="26">
         <v>1.76</v>
       </c>
-      <c r="F31" s="28">
+      <c r="F31" s="27">
         <v>359</v>
+      </c>
+      <c r="G31" s="1">
+        <v>4102.4063476562496</v>
       </c>
       <c r="H31" s="1" t="s">
         <v>24</v>
@@ -2053,8 +2205,21 @@
       <c r="I31" s="1" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="32" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="J31" s="4">
+        <f>E31*G31/62.5</f>
+        <v>115.52376274999999</v>
+      </c>
+      <c r="K31" s="5">
+        <f>G31/G30</f>
+        <v>0.23978482049510644</v>
+      </c>
+      <c r="L31" s="5">
+        <f>J31/J30</f>
+        <v>0.40578969622248778</v>
+      </c>
+      <c r="M31" s="5"/>
+    </row>
+    <row r="32" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A32" s="1">
         <v>30</v>
       </c>
@@ -2065,14 +2230,17 @@
         <v>26</v>
       </c>
       <c r="D32" s="1" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>C5</v>
       </c>
-      <c r="E32" s="29">
+      <c r="E32" s="28">
         <v>0.91800000000000004</v>
       </c>
-      <c r="F32" s="28">
+      <c r="F32" s="27">
         <v>95</v>
+      </c>
+      <c r="G32" s="1">
+        <v>9296.0865478515625</v>
       </c>
       <c r="H32" s="1" t="s">
         <v>28</v>
@@ -2080,8 +2248,13 @@
       <c r="I32" s="1" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J32" s="4">
+        <f t="shared" ref="J32:J36" si="3">E32*G32/62.5</f>
+        <v>136.54091921484374</v>
+      </c>
+      <c r="K32" s="4"/>
+    </row>
+    <row r="33" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A33" s="1">
         <v>31</v>
       </c>
@@ -2092,14 +2265,17 @@
         <v>30</v>
       </c>
       <c r="D33" s="1" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>D5</v>
       </c>
-      <c r="E33" s="29">
+      <c r="E33" s="28">
         <v>0.71499999999999997</v>
       </c>
-      <c r="F33" s="28">
+      <c r="F33" s="27">
         <v>48</v>
+      </c>
+      <c r="G33" s="1">
+        <v>7447.2508789062504</v>
       </c>
       <c r="H33" s="1" t="s">
         <v>32</v>
@@ -2107,8 +2283,22 @@
       <c r="I33" s="1" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J33" s="4">
+        <f t="shared" si="3"/>
+        <v>85.196550054687492</v>
+      </c>
+      <c r="K33" s="4"/>
+      <c r="M33" s="5">
+        <f>(G32-G33)/G32</f>
+        <v>0.19888322461591112</v>
+      </c>
+      <c r="N33" s="5">
+        <f>(J32-J33)/J32</f>
+        <v>0.37603649847535564</v>
+      </c>
+      <c r="O33" s="5"/>
+    </row>
+    <row r="34" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A34" s="1">
         <v>32</v>
       </c>
@@ -2119,14 +2309,17 @@
         <v>34</v>
       </c>
       <c r="D34" s="1" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>E5</v>
       </c>
-      <c r="E34" s="29">
+      <c r="E34" s="28">
         <v>0.79300000000000004</v>
       </c>
-      <c r="F34" s="28">
+      <c r="F34" s="27">
         <v>190</v>
+      </c>
+      <c r="G34" s="1">
+        <v>8289.4</v>
       </c>
       <c r="H34" s="1" t="s">
         <v>36</v>
@@ -2134,8 +2327,13 @@
       <c r="I34" s="1" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J34" s="4">
+        <f t="shared" si="3"/>
+        <v>105.1759072</v>
+      </c>
+      <c r="K34" s="4"/>
+    </row>
+    <row r="35" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A35" s="1">
         <v>33</v>
       </c>
@@ -2146,14 +2344,17 @@
         <v>38</v>
       </c>
       <c r="D35" s="1" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>F5</v>
       </c>
-      <c r="E35" s="29">
+      <c r="E35" s="28">
         <v>0.44700000000000001</v>
       </c>
-      <c r="F35" s="28">
+      <c r="F35" s="27">
         <v>52</v>
+      </c>
+      <c r="G35" s="1">
+        <v>4973.94677734375</v>
       </c>
       <c r="H35" s="1" t="s">
         <v>40</v>
@@ -2161,8 +2362,13 @@
       <c r="I35" s="1" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J35" s="4">
+        <f t="shared" si="3"/>
+        <v>35.573667351562499</v>
+      </c>
+      <c r="K35" s="4"/>
+    </row>
+    <row r="36" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A36" s="1">
         <v>34</v>
       </c>
@@ -2173,20 +2379,39 @@
         <v>42</v>
       </c>
       <c r="D36" s="1" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>G5</v>
       </c>
-      <c r="E36" s="27">
+      <c r="E36" s="26">
         <v>1.27</v>
       </c>
-      <c r="F36" s="28">
+      <c r="F36" s="27">
         <v>330</v>
+      </c>
+      <c r="G36" s="1">
+        <v>3301.4569335937499</v>
       </c>
       <c r="H36" s="9" t="s">
         <v>44</v>
       </c>
       <c r="I36" s="9" t="s">
         <v>45</v>
+      </c>
+      <c r="J36" s="11">
+        <f t="shared" si="3"/>
+        <v>67.085604890624992</v>
+      </c>
+      <c r="K36" s="11"/>
+      <c r="L36" s="9"/>
+      <c r="M36" s="9"/>
+      <c r="N36" s="9"/>
+      <c r="O36" s="12">
+        <f>G36/G34</f>
+        <v>0.39827453538178276</v>
+      </c>
+      <c r="P36" s="12">
+        <f>J36/J34</f>
+        <v>0.6378419419102952</v>
       </c>
     </row>
   </sheetData>
@@ -2197,120 +2422,243 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ECA2F88A-A2D5-4C5A-A713-359268450BDA}">
-  <dimension ref="B2:H6"/>
+  <dimension ref="B2:L10"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="K11" sqref="K11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="4.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.88671875" style="1" customWidth="1"/>
-    <col min="4" max="4" width="10.33203125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="4.6640625" style="1" customWidth="1"/>
-    <col min="6" max="6" width="6.33203125" style="1" customWidth="1"/>
-    <col min="7" max="7" width="5.109375" style="1" customWidth="1"/>
-    <col min="8" max="8" width="8.88671875" style="1"/>
+    <col min="3" max="3" width="4.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.88671875" style="1" customWidth="1"/>
+    <col min="5" max="5" width="10.33203125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="4.6640625" style="1" customWidth="1"/>
+    <col min="7" max="7" width="6.33203125" style="1" customWidth="1"/>
+    <col min="8" max="8" width="5.109375" style="1" customWidth="1"/>
+    <col min="9" max="9" width="2.33203125" style="1" customWidth="1"/>
+    <col min="10" max="10" width="6.77734375" style="1" customWidth="1"/>
+    <col min="11" max="11" width="7.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B2" s="20"/>
-      <c r="C2" s="20" t="s">
+    <row r="2" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="C2" s="20"/>
+      <c r="D2" s="20" t="s">
         <v>88</v>
       </c>
-      <c r="D2" s="24" t="s">
+      <c r="E2" s="24" t="s">
         <v>89</v>
       </c>
-      <c r="E2" s="26" t="s">
+      <c r="F2" s="42" t="s">
         <v>90</v>
       </c>
-      <c r="F2" s="26"/>
-      <c r="G2" s="26"/>
-    </row>
-    <row r="3" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="G2" s="42"/>
+      <c r="H2" s="42"/>
+      <c r="I2" s="31"/>
+      <c r="J2" s="42" t="s">
+        <v>87</v>
+      </c>
+      <c r="K2" s="42"/>
+    </row>
+    <row r="3" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B3" s="21" t="s">
+        <v>95</v>
+      </c>
+      <c r="C3" s="21" t="s">
         <v>66</v>
       </c>
-      <c r="C3" s="21" t="s">
+      <c r="D3" s="21" t="s">
         <v>91</v>
       </c>
-      <c r="D3" s="21" t="s">
+      <c r="E3" s="21" t="s">
         <v>92</v>
       </c>
-      <c r="E3" s="21" t="s">
+      <c r="F3" s="21" t="s">
         <v>80</v>
       </c>
-      <c r="F3" s="21" t="s">
+      <c r="G3" s="21" t="s">
         <v>81</v>
       </c>
-      <c r="G3" s="21" t="s">
+      <c r="H3" s="21" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="4" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B4" s="1">
+      <c r="I3" s="21"/>
+      <c r="J3" s="21" t="s">
+        <v>79</v>
+      </c>
+      <c r="K3" s="21" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B4" s="40">
+        <v>44230</v>
+      </c>
+      <c r="C4" s="1">
         <v>1</v>
       </c>
-      <c r="C4" s="19">
+      <c r="D4" s="19">
         <v>996.9782399999998</v>
       </c>
-      <c r="D4" s="23">
+      <c r="E4" s="23">
         <v>1.3</v>
       </c>
-      <c r="E4" s="22">
+      <c r="F4" s="22">
         <v>25</v>
       </c>
-      <c r="F4" s="22">
+      <c r="G4" s="22">
         <v>22</v>
       </c>
-      <c r="G4" s="22">
+      <c r="H4" s="22">
         <v>42</v>
       </c>
-    </row>
-    <row r="5" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B5" s="1">
+      <c r="I4" s="22"/>
+      <c r="J4" s="19">
+        <f>'FAR-csf'!F14</f>
+        <v>32.018108912532774</v>
+      </c>
+      <c r="K4" s="19">
+        <f>'FAR-csf'!G14</f>
+        <v>59.400998287645145</v>
+      </c>
+    </row>
+    <row r="5" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B5" s="40">
+        <v>44230</v>
+      </c>
+      <c r="C5" s="1">
         <v>2</v>
       </c>
-      <c r="C5" s="19">
+      <c r="D5" s="19">
         <v>972.85536000000002</v>
       </c>
-      <c r="D5" s="23">
+      <c r="E5" s="23">
         <v>1.55</v>
       </c>
-      <c r="E5" s="22">
+      <c r="F5" s="22">
         <v>25</v>
       </c>
-      <c r="F5" s="22">
+      <c r="G5" s="22">
         <v>22</v>
       </c>
-      <c r="G5" s="22">
+      <c r="H5" s="22">
         <v>42</v>
       </c>
-    </row>
-    <row r="6" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B6" s="1">
+      <c r="I5" s="22"/>
+      <c r="J5" s="19">
+        <f>'FAR-csf'!F15</f>
+        <v>31.927264215838612</v>
+      </c>
+      <c r="K5" s="19">
+        <f>'FAR-csf'!G15</f>
+        <v>60.554081661965562</v>
+      </c>
+    </row>
+    <row r="6" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B6" s="41">
+        <v>44230</v>
+      </c>
+      <c r="C6" s="9">
         <v>3</v>
       </c>
-      <c r="C6" s="19">
+      <c r="D6" s="33">
         <v>856.45728000000008</v>
       </c>
-      <c r="D6" s="23">
+      <c r="E6" s="34">
         <v>1</v>
       </c>
-      <c r="E6" s="22">
+      <c r="F6" s="35">
         <v>25</v>
       </c>
-      <c r="F6" s="22">
+      <c r="G6" s="35">
         <v>22</v>
       </c>
-      <c r="G6" s="22">
+      <c r="H6" s="35">
         <v>38</v>
       </c>
+      <c r="I6" s="35"/>
+      <c r="J6" s="33">
+        <f>'FAR-csf'!F16</f>
+        <v>31.426790956901112</v>
+      </c>
+      <c r="K6" s="33">
+        <f>'FAR-csf'!G16</f>
+        <v>51.300016366594406</v>
+      </c>
+    </row>
+    <row r="7" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B7" s="40">
+        <v>44250</v>
+      </c>
+      <c r="C7" s="32">
+        <v>4</v>
+      </c>
+      <c r="D7" s="1">
+        <v>981</v>
+      </c>
+      <c r="E7" s="25">
+        <v>1.2</v>
+      </c>
+      <c r="F7" s="1">
+        <v>24</v>
+      </c>
+      <c r="G7" s="1">
+        <v>20</v>
+      </c>
+      <c r="H7" s="1">
+        <v>40</v>
+      </c>
+      <c r="J7" s="19">
+        <f>'FAR-csf'!F23</f>
+        <v>30.080000000000002</v>
+      </c>
+      <c r="K7" s="19">
+        <f>'FAR-csf'!G23</f>
+        <v>56.761981000000006</v>
+      </c>
+    </row>
+    <row r="8" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B8" s="40">
+        <v>44250</v>
+      </c>
+      <c r="C8" s="32">
+        <v>5</v>
+      </c>
+      <c r="D8" s="1">
+        <v>854</v>
+      </c>
+      <c r="E8" s="25">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="F8" s="1">
+        <v>24</v>
+      </c>
+      <c r="G8" s="1">
+        <v>20</v>
+      </c>
+      <c r="H8" s="1">
+        <v>40</v>
+      </c>
+      <c r="J8" s="19">
+        <f>'FAR-csf'!F24</f>
+        <v>30.080000000000002</v>
+      </c>
+      <c r="K8" s="19">
+        <f>'FAR-csf'!G24</f>
+        <v>54.849347199999997</v>
+      </c>
+      <c r="L8" s="1"/>
+    </row>
+    <row r="9" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="L9" s="1"/>
+    </row>
+    <row r="10" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="L10" s="1"/>
     </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="E2:G2"/>
+  <mergeCells count="2">
+    <mergeCell ref="F2:H2"/>
+    <mergeCell ref="J2:K2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
@@ -2319,10 +2667,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:X22"/>
+  <dimension ref="A1:X36"/>
   <sheetViews>
     <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3281,6 +3629,118 @@
         <v>118</v>
       </c>
     </row>
+    <row r="23" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A23" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="24" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A24" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="25" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A25" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="26" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A26" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="27" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A27" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="28" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A28" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="29" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A29" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="B29" s="9" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="30" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A30" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="31" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A31" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="32" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A32" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A33" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A34" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A35" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A36" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="B36" s="9" t="s">
+        <v>45</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
@@ -3291,7 +3751,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:S20"/>
   <sheetViews>
-    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0"/>
+    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -3543,6 +4005,9 @@
       </c>
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A5" s="1">
+        <v>4</v>
+      </c>
       <c r="D5" s="1"/>
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
@@ -3557,6 +4022,9 @@
       <c r="O5" s="1"/>
     </row>
     <row r="6" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A6" s="1">
+        <v>5</v>
+      </c>
       <c r="D6" s="17"/>
       <c r="E6" s="17"/>
       <c r="F6" s="17"/>
@@ -3752,16 +4220,18 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:H10"/>
+  <dimension ref="A1:H16"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="3" max="3" width="9.109375" customWidth="1"/>
     <col min="4" max="5" width="8.88671875" style="1" customWidth="1"/>
+    <col min="16" max="16" width="9.88671875" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="11.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.3">
@@ -3951,6 +4421,114 @@
       </c>
       <c r="G10" s="4"/>
       <c r="H10" s="4"/>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A11" s="1">
+        <v>4</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="C11" s="25">
+        <f>out!E23</f>
+        <v>1.24</v>
+      </c>
+      <c r="D11" s="1">
+        <v>24</v>
+      </c>
+      <c r="E11" s="1">
+        <v>39.5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A12" s="1">
+        <v>4</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="C12" s="25">
+        <f>out!E25</f>
+        <v>1.01</v>
+      </c>
+      <c r="D12" s="1">
+        <v>20</v>
+      </c>
+      <c r="E12" s="1">
+        <v>43.1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A13" s="1">
+        <v>4</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="C13" s="1">
+        <f>out!E27</f>
+        <v>0.82399999999999995</v>
+      </c>
+      <c r="D13" s="1">
+        <v>40</v>
+      </c>
+      <c r="E13" s="1">
+        <v>66.2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A14" s="1">
+        <v>5</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="C14" s="25">
+        <f>out!E30</f>
+        <v>1.04</v>
+      </c>
+      <c r="D14" s="1">
+        <v>24</v>
+      </c>
+      <c r="E14" s="1">
+        <v>40.6</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A15" s="1">
+        <v>5</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="C15" s="1">
+        <f>out!E32</f>
+        <v>0.91800000000000004</v>
+      </c>
+      <c r="D15" s="1">
+        <v>20</v>
+      </c>
+      <c r="E15" s="1">
+        <v>37.6</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A16" s="1">
+        <v>5</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="C16" s="1">
+        <f>out!E34</f>
+        <v>0.79300000000000004</v>
+      </c>
+      <c r="D16" s="1">
+        <v>40</v>
+      </c>
+      <c r="E16" s="1">
+        <v>63.8</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
@@ -3960,10 +4538,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="A1:AMJ18"/>
+  <dimension ref="A1:AMG31"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J23" sqref="J23"/>
+      <selection activeCell="L13" sqref="L13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3972,7 +4550,10 @@
     <col min="2" max="2" width="9.88671875" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="5" width="8.88671875" style="1"/>
     <col min="6" max="7" width="9.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="1024" width="8.88671875" style="1"/>
+    <col min="8" max="14" width="8.88671875" style="1"/>
+    <col min="15" max="15" width="14" style="1" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="10.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="17" max="1021" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.3">
@@ -4423,7 +5004,7 @@
         <v>60.554081661965562</v>
       </c>
       <c r="H15" s="19">
-        <f t="shared" ref="H15:H16" si="4">C15-D15</f>
+        <f t="shared" ref="H15:H24" si="4">C15-D15</f>
         <v>153</v>
       </c>
     </row>
@@ -4457,11 +5038,316 @@
         <v>112</v>
       </c>
     </row>
-    <row r="17" spans="4:4" x14ac:dyDescent="0.3">
-      <c r="D17" s="4"/>
-    </row>
-    <row r="18" spans="4:4" x14ac:dyDescent="0.3">
-      <c r="D18" s="4"/>
+    <row r="17" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A17" s="1">
+        <v>4</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="C17" s="1">
+        <v>196</v>
+      </c>
+      <c r="D17" s="4">
+        <v>90</v>
+      </c>
+      <c r="E17" s="1">
+        <v>347</v>
+      </c>
+      <c r="F17" s="1">
+        <v>24</v>
+      </c>
+      <c r="G17" s="25">
+        <v>39.5</v>
+      </c>
+      <c r="H17" s="19">
+        <f t="shared" si="4"/>
+        <v>106</v>
+      </c>
+      <c r="J17" s="37"/>
+      <c r="K17" s="37"/>
+      <c r="L17" s="37"/>
+    </row>
+    <row r="18" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A18" s="1">
+        <v>4</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="C18" s="4">
+        <v>90</v>
+      </c>
+      <c r="D18" s="4">
+        <v>41</v>
+      </c>
+      <c r="E18" s="1">
+        <v>184</v>
+      </c>
+      <c r="F18" s="1">
+        <v>20</v>
+      </c>
+      <c r="G18" s="25">
+        <v>43.1</v>
+      </c>
+      <c r="H18" s="19">
+        <f t="shared" si="4"/>
+        <v>49</v>
+      </c>
+      <c r="J18" s="38"/>
+      <c r="K18" s="38"/>
+      <c r="L18" s="38"/>
+    </row>
+    <row r="19" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A19" s="1">
+        <v>4</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="C19" s="1">
+        <v>184</v>
+      </c>
+      <c r="D19" s="1">
+        <v>46</v>
+      </c>
+      <c r="E19" s="1">
+        <v>320</v>
+      </c>
+      <c r="F19" s="1">
+        <v>40</v>
+      </c>
+      <c r="G19" s="25">
+        <v>66.2</v>
+      </c>
+      <c r="H19" s="19">
+        <f t="shared" si="4"/>
+        <v>138</v>
+      </c>
+      <c r="J19" s="38"/>
+      <c r="K19" s="38"/>
+      <c r="L19" s="38"/>
+    </row>
+    <row r="20" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A20" s="1">
+        <v>5</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="C20" s="1">
+        <v>166</v>
+      </c>
+      <c r="D20" s="1">
+        <v>95</v>
+      </c>
+      <c r="E20" s="1">
+        <v>359</v>
+      </c>
+      <c r="F20" s="1">
+        <v>24</v>
+      </c>
+      <c r="G20" s="25">
+        <v>40.6</v>
+      </c>
+      <c r="H20" s="19">
+        <f t="shared" si="4"/>
+        <v>71</v>
+      </c>
+      <c r="J20" s="38"/>
+      <c r="K20" s="38"/>
+      <c r="L20" s="38"/>
+    </row>
+    <row r="21" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A21" s="1">
+        <v>5</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="C21" s="4">
+        <v>95</v>
+      </c>
+      <c r="D21" s="1">
+        <v>48</v>
+      </c>
+      <c r="E21" s="1">
+        <v>190</v>
+      </c>
+      <c r="F21" s="1">
+        <v>20</v>
+      </c>
+      <c r="G21" s="25">
+        <v>37.6</v>
+      </c>
+      <c r="H21" s="19">
+        <f t="shared" si="4"/>
+        <v>47</v>
+      </c>
+      <c r="J21" s="38"/>
+      <c r="K21" s="38"/>
+      <c r="L21" s="38"/>
+    </row>
+    <row r="22" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A22" s="1">
+        <v>5</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="C22" s="1">
+        <v>190</v>
+      </c>
+      <c r="D22" s="1">
+        <v>52</v>
+      </c>
+      <c r="E22" s="1">
+        <v>330</v>
+      </c>
+      <c r="F22" s="1">
+        <v>40</v>
+      </c>
+      <c r="G22" s="25">
+        <v>63.8</v>
+      </c>
+      <c r="H22" s="19">
+        <f t="shared" si="4"/>
+        <v>138</v>
+      </c>
+      <c r="J22" s="38"/>
+      <c r="K22" s="38"/>
+      <c r="L22" s="38"/>
+    </row>
+    <row r="23" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A23" s="1">
+        <v>4</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="C23" s="1">
+        <f>C17</f>
+        <v>196</v>
+      </c>
+      <c r="D23" s="39">
+        <f>AVERAGE(D18,D19)</f>
+        <v>43.5</v>
+      </c>
+      <c r="E23" s="25">
+        <f>AVERAGE(E17,E19)</f>
+        <v>333.5</v>
+      </c>
+      <c r="F23" s="1">
+        <v>30.080000000000002</v>
+      </c>
+      <c r="G23" s="25">
+        <v>56.761981000000006</v>
+      </c>
+      <c r="H23" s="19">
+        <f t="shared" si="4"/>
+        <v>152.5</v>
+      </c>
+      <c r="J23" s="38"/>
+      <c r="K23" s="38"/>
+      <c r="L23" s="38"/>
+    </row>
+    <row r="24" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A24" s="1">
+        <v>5</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="C24" s="1">
+        <f>C20</f>
+        <v>166</v>
+      </c>
+      <c r="D24" s="39">
+        <f>AVERAGE(D21:D22)</f>
+        <v>50</v>
+      </c>
+      <c r="E24" s="25">
+        <f>AVERAGE(E20,E22)</f>
+        <v>344.5</v>
+      </c>
+      <c r="F24" s="1">
+        <v>30.080000000000002</v>
+      </c>
+      <c r="G24" s="25">
+        <v>54.849347199999997</v>
+      </c>
+      <c r="H24" s="19">
+        <f t="shared" si="4"/>
+        <v>116</v>
+      </c>
+      <c r="J24" s="38"/>
+      <c r="K24" s="38"/>
+      <c r="L24" s="38"/>
+    </row>
+    <row r="25" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="J25" s="38"/>
+      <c r="K25" s="38"/>
+      <c r="L25" s="38"/>
+    </row>
+    <row r="26" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="J26" s="38"/>
+      <c r="K26" s="38"/>
+      <c r="L26" s="38"/>
+      <c r="M26" s="38"/>
+      <c r="N26" s="38"/>
+      <c r="O26" s="38"/>
+      <c r="P26" s="38"/>
+      <c r="Q26" s="38"/>
+    </row>
+    <row r="27" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="J27" s="38"/>
+      <c r="K27" s="38"/>
+      <c r="L27" s="38"/>
+      <c r="M27" s="38"/>
+      <c r="N27" s="38"/>
+      <c r="O27" s="38"/>
+      <c r="P27" s="38"/>
+      <c r="Q27" s="38"/>
+    </row>
+    <row r="28" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="J28" s="38"/>
+      <c r="K28" s="38"/>
+      <c r="L28" s="38"/>
+      <c r="M28" s="38"/>
+      <c r="N28" s="38"/>
+      <c r="O28" s="38"/>
+      <c r="P28" s="38"/>
+      <c r="Q28" s="38"/>
+    </row>
+    <row r="29" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="J29" s="38"/>
+      <c r="K29" s="38"/>
+      <c r="L29" s="38"/>
+      <c r="M29" s="38"/>
+      <c r="N29" s="38"/>
+      <c r="O29" s="38"/>
+      <c r="P29" s="38"/>
+      <c r="Q29" s="38"/>
+    </row>
+    <row r="30" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="J30" s="38"/>
+      <c r="K30" s="38"/>
+      <c r="L30" s="38"/>
+      <c r="M30" s="38"/>
+      <c r="N30" s="38"/>
+      <c r="O30" s="38"/>
+      <c r="P30" s="38"/>
+      <c r="Q30" s="38"/>
+    </row>
+    <row r="31" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="J31" s="38"/>
+      <c r="K31" s="38"/>
+      <c r="L31" s="38"/>
+      <c r="M31" s="38"/>
+      <c r="N31" s="38"/>
+      <c r="O31" s="38"/>
+      <c r="P31" s="38"/>
+      <c r="Q31" s="38"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
@@ -4471,22 +5357,22 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
-  <dimension ref="A1:AMJ18"/>
+  <dimension ref="A1:AMK24"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H26" sqref="H26"/>
+      <selection activeCell="G28" sqref="G28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="8.88671875" style="1"/>
-    <col min="2" max="2" width="10.33203125" style="1" customWidth="1"/>
-    <col min="3" max="17" width="8.88671875" style="1"/>
-    <col min="18" max="18" width="17.109375" style="1" customWidth="1"/>
-    <col min="19" max="1024" width="8.88671875" style="1"/>
+    <col min="2" max="3" width="10.33203125" style="1" customWidth="1"/>
+    <col min="4" max="18" width="8.88671875" style="1"/>
+    <col min="19" max="19" width="17.109375" style="1" customWidth="1"/>
+    <col min="20" max="1025" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>66</v>
       </c>
@@ -4494,464 +5380,675 @@
         <v>77</v>
       </c>
       <c r="C1" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="G1" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="H1" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="H1" s="21" t="s">
+      <c r="I1" s="21" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="C2" s="1">
+      <c r="D2" s="1">
         <f>out!E2</f>
         <v>1.38</v>
       </c>
-      <c r="D2" s="1">
+      <c r="E2" s="1">
         <f>out!E4</f>
         <v>1.08</v>
       </c>
-      <c r="E2" s="1">
+      <c r="F2" s="1">
         <f>out!E3</f>
         <v>2.2799999999999998</v>
       </c>
-      <c r="F2" s="4">
+      <c r="G2" s="4">
         <v>25.081389940867702</v>
       </c>
-      <c r="G2" s="4">
+      <c r="H2" s="4">
         <v>41.438818163172797</v>
       </c>
-      <c r="H2" s="19">
+      <c r="I2" s="19">
         <v>41</v>
       </c>
-      <c r="R2" s="4"/>
-    </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S2" s="4"/>
+    </row>
+    <row r="3" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="C3" s="1">
+      <c r="D3" s="1">
         <f>out!E9</f>
         <v>1.62</v>
       </c>
-      <c r="D3" s="1">
+      <c r="E3" s="1">
         <f>out!E11</f>
         <v>1.34</v>
       </c>
-      <c r="E3" s="1">
+      <c r="F3" s="1">
         <f>out!E10</f>
         <v>2.61</v>
       </c>
-      <c r="F3" s="4">
+      <c r="G3" s="4">
         <v>25.025977140116701</v>
       </c>
-      <c r="G3" s="4">
+      <c r="H3" s="4">
         <v>40.319629836854702</v>
       </c>
-      <c r="H3" s="19">
+      <c r="I3" s="19">
         <v>91</v>
       </c>
-      <c r="R3" s="4"/>
-    </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S3" s="4"/>
+    </row>
+    <row r="4" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="C4" s="1">
+      <c r="D4" s="1">
         <f>out!E16</f>
         <v>0.98</v>
       </c>
-      <c r="D4" s="1">
+      <c r="E4" s="1">
         <f>out!E18</f>
         <v>0.8</v>
       </c>
-      <c r="E4" s="1">
+      <c r="F4" s="1">
         <f>out!E17</f>
         <v>1.39</v>
       </c>
-      <c r="F4" s="4">
+      <c r="G4" s="4">
         <v>25.1222057450431</v>
       </c>
-      <c r="G4" s="4">
+      <c r="H4" s="4">
         <v>35.632516311846899</v>
       </c>
-      <c r="H4" s="19">
+      <c r="I4" s="19">
         <v>71</v>
       </c>
-      <c r="R4" s="4"/>
-    </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S4" s="4"/>
+    </row>
+    <row r="5" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
         <v>1</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="C5" s="1">
-        <f>D2</f>
+      <c r="D5" s="1">
+        <f>E2</f>
         <v>1.08</v>
       </c>
-      <c r="D5" s="1">
+      <c r="E5" s="1">
         <f>out!E5</f>
         <v>0.78</v>
       </c>
-      <c r="E5" s="1">
+      <c r="F5" s="1">
         <f>out!E6</f>
         <v>0.91</v>
       </c>
-      <c r="F5" s="4">
+      <c r="G5" s="4">
         <v>22.027475130269998</v>
       </c>
-      <c r="G5" s="4">
+      <c r="H5" s="4">
         <v>43.686509816306099</v>
       </c>
-      <c r="H5" s="19">
+      <c r="I5" s="19">
         <v>82</v>
       </c>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
         <v>2</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="C6" s="1">
-        <f>D3</f>
+      <c r="D6" s="1">
+        <f>E3</f>
         <v>1.34</v>
       </c>
-      <c r="D6" s="1">
+      <c r="E6" s="1">
         <f>out!E12</f>
         <v>0.91</v>
       </c>
-      <c r="E6" s="1">
+      <c r="F6" s="1">
         <f>out!E13</f>
         <v>1.1200000000000001</v>
       </c>
-      <c r="F6" s="4">
+      <c r="G6" s="4">
         <v>22.0036790717419</v>
       </c>
-      <c r="G6" s="4">
+      <c r="H6" s="4">
         <v>47.032349220362001</v>
       </c>
-      <c r="H6" s="19">
+      <c r="I6" s="19">
         <v>62</v>
       </c>
     </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
         <v>3</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="C7" s="1">
-        <f>D4</f>
+      <c r="D7" s="1">
+        <f>E4</f>
         <v>0.8</v>
       </c>
-      <c r="D7" s="1">
+      <c r="E7" s="1">
         <f>out!E19</f>
         <v>0.6</v>
       </c>
-      <c r="E7" s="1">
+      <c r="F7" s="1">
         <f>out!E20</f>
         <v>0.64</v>
       </c>
-      <c r="F7" s="4">
+      <c r="G7" s="4">
         <v>21.969909354266001</v>
       </c>
-      <c r="G7" s="4">
+      <c r="H7" s="4">
         <v>41.477432015699499</v>
       </c>
-      <c r="H7" s="19">
+      <c r="I7" s="19">
         <v>46</v>
       </c>
     </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
         <v>1</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="C8" s="1">
-        <f>E5</f>
+      <c r="D8" s="1">
+        <f>F5</f>
         <v>0.91</v>
       </c>
-      <c r="D8" s="1">
+      <c r="E8" s="1">
         <f>out!E7</f>
         <v>0.46</v>
       </c>
-      <c r="E8" s="1">
+      <c r="F8" s="1">
         <f>out!E8</f>
         <v>1.52</v>
       </c>
-      <c r="F8" s="4">
+      <c r="G8" s="4">
         <v>42.033898305084698</v>
       </c>
-      <c r="G8" s="4">
+      <c r="H8" s="4">
         <v>70.210467498603094</v>
       </c>
-      <c r="H8" s="19">
+      <c r="I8" s="19">
         <v>109</v>
       </c>
     </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
         <v>2</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="C9" s="1">
-        <f>E6</f>
+      <c r="D9" s="1">
+        <f>F6</f>
         <v>1.1200000000000001</v>
       </c>
-      <c r="D9" s="1">
+      <c r="E9" s="1">
         <f>out!E14</f>
         <v>0.52</v>
       </c>
-      <c r="E9" s="1">
+      <c r="F9" s="1">
         <f>out!E15</f>
         <v>1.93</v>
       </c>
-      <c r="F9" s="4">
+      <c r="G9" s="4">
         <v>41.833478387003197</v>
       </c>
-      <c r="G9" s="4">
+      <c r="H9" s="4">
         <v>72.088047577603703</v>
       </c>
-      <c r="H9" s="19">
+      <c r="I9" s="19">
         <v>176</v>
       </c>
     </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
         <v>3</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="C10" s="1">
-        <f>E7</f>
+      <c r="D10" s="1">
+        <f>F7</f>
         <v>0.64</v>
       </c>
-      <c r="D10" s="1">
+      <c r="E10" s="1">
         <f>out!E21</f>
         <v>0.39</v>
       </c>
-      <c r="E10" s="1">
+      <c r="F10" s="1">
         <f>out!E22</f>
         <v>0.98</v>
       </c>
-      <c r="F10" s="4">
+      <c r="G10" s="4">
         <v>38.324386503067501</v>
       </c>
-      <c r="G10" s="4">
+      <c r="H10" s="4">
         <v>58.684216832822102</v>
       </c>
-      <c r="H10" s="19">
+      <c r="I10" s="19">
         <v>118</v>
       </c>
     </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>86</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="C11" s="4">
-        <f>_xlfn.STDEV.P(C2:C4)</f>
-        <v>0.26398653164297781</v>
-      </c>
       <c r="D11" s="4">
         <f>_xlfn.STDEV.P(D2:D4)</f>
-        <v>0.22050447211388433</v>
+        <v>0.26398653164297781</v>
       </c>
       <c r="E11" s="4">
         <f>_xlfn.STDEV.P(E2:E4)</f>
-        <v>0.51525613910839441</v>
+        <v>0.22050447211388433</v>
       </c>
       <c r="F11" s="4">
         <f>_xlfn.STDEV.P(F2:F4)</f>
-        <v>3.943553496761161E-2</v>
+        <v>0.51525613910839441</v>
       </c>
       <c r="G11" s="4">
         <f>_xlfn.STDEV.P(G2:G4)</f>
+        <v>3.943553496761161E-2</v>
+      </c>
+      <c r="H11" s="4">
+        <f>_xlfn.STDEV.P(H2:H4)</f>
         <v>2.5151707893144999</v>
       </c>
-      <c r="H11" s="19">
+      <c r="I11" s="19">
         <v>18.19732762431795</v>
       </c>
     </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>86</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="C12" s="4">
-        <f>_xlfn.STDEV.P(C5:C7)</f>
-        <v>0.22050447211388433</v>
-      </c>
       <c r="D12" s="4">
         <f>_xlfn.STDEV.P(D5:D7)</f>
-        <v>0.12710450643291726</v>
+        <v>0.22050447211388433</v>
       </c>
       <c r="E12" s="4">
         <f>_xlfn.STDEV.P(E5:E7)</f>
-        <v>0.19646882704388513</v>
+        <v>0.12710450643291726</v>
       </c>
       <c r="F12" s="4">
         <f>_xlfn.STDEV.P(F5:F7)</f>
-        <v>2.3618412748477768E-2</v>
+        <v>0.19646882704388513</v>
       </c>
       <c r="G12" s="4">
         <f>_xlfn.STDEV.P(G5:G7)</f>
+        <v>2.3618412748477768E-2</v>
+      </c>
+      <c r="H12" s="4">
+        <f>_xlfn.STDEV.P(H5:H7)</f>
         <v>2.2835588987738102</v>
       </c>
-      <c r="H12" s="19">
+      <c r="I12" s="19">
         <v>-10.293878958713464</v>
       </c>
     </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>86</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="C13" s="4">
-        <f>_xlfn.STDEV.P(C8:C10)</f>
-        <v>0.19646882704388513</v>
-      </c>
       <c r="D13" s="4">
         <f>_xlfn.STDEV.P(D8:D10)</f>
-        <v>5.3124591501697516E-2</v>
+        <v>0.19646882704388513</v>
       </c>
       <c r="E13" s="4">
         <f>_xlfn.STDEV.P(E8:E10)</f>
-        <v>0.38904441334577178</v>
+        <v>5.3124591501697516E-2</v>
       </c>
       <c r="F13" s="4">
         <f>_xlfn.STDEV.P(F8:F10)</f>
-        <v>1.703407428354905</v>
+        <v>0.38904441334577178</v>
       </c>
       <c r="G13" s="4">
         <f>_xlfn.STDEV.P(G8:G10)</f>
+        <v>1.703407428354905</v>
+      </c>
+      <c r="H13" s="4">
+        <f>_xlfn.STDEV.P(H8:H10)</f>
         <v>5.9258608375889077</v>
       </c>
-      <c r="H13" s="19">
+      <c r="I13" s="19">
         <v>18.907097433455025</v>
       </c>
     </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A14" s="1">
         <v>1</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="C14" s="1">
-        <f>C2</f>
+      <c r="D14" s="1">
+        <f>D2</f>
         <v>1.38</v>
       </c>
-      <c r="D14" s="4">
-        <f>AVERAGE(D5,D8)</f>
+      <c r="E14" s="4">
+        <f>AVERAGE(E5,E8)</f>
         <v>0.62</v>
       </c>
-      <c r="E14" s="25">
-        <f>AVERAGE(E2,E8)</f>
+      <c r="F14" s="25">
+        <f>AVERAGE(F2,F8)</f>
         <v>1.9</v>
       </c>
-      <c r="G14" s="4">
+      <c r="H14" s="4">
         <v>59.400998287645102</v>
       </c>
-      <c r="H14" s="19">
+      <c r="I14" s="19">
         <v>117</v>
       </c>
     </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A15" s="1">
         <v>2</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="C15" s="1">
-        <f>C3</f>
+      <c r="D15" s="1">
+        <f>D3</f>
         <v>1.62</v>
       </c>
-      <c r="D15" s="4">
-        <f t="shared" ref="D15:D16" si="0">AVERAGE(D6,D9)</f>
+      <c r="E15" s="4">
+        <f t="shared" ref="E15:E16" si="0">AVERAGE(E6,E9)</f>
         <v>0.71500000000000008</v>
       </c>
-      <c r="E15" s="25">
-        <f t="shared" ref="E15:E16" si="1">AVERAGE(E3,E9)</f>
+      <c r="F15" s="25">
+        <f t="shared" ref="F15:F16" si="1">AVERAGE(F3,F9)</f>
         <v>2.27</v>
       </c>
-      <c r="G15" s="4">
+      <c r="H15" s="4">
         <v>60.554081661965597</v>
       </c>
-      <c r="H15" s="19">
+      <c r="I15" s="19">
         <v>153</v>
       </c>
     </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A16" s="1">
         <v>3</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="C16" s="1">
-        <f>C4</f>
+      <c r="D16" s="1">
+        <f>D4</f>
         <v>0.98</v>
       </c>
-      <c r="D16" s="4">
+      <c r="E16" s="4">
         <f t="shared" si="0"/>
         <v>0.495</v>
       </c>
-      <c r="E16" s="25">
+      <c r="F16" s="25">
         <f t="shared" si="1"/>
         <v>1.1850000000000001</v>
       </c>
-      <c r="G16" s="4">
+      <c r="H16" s="4">
         <v>51.300016366594399</v>
       </c>
-      <c r="H16" s="19">
+      <c r="I16" s="19">
         <v>112</v>
       </c>
     </row>
-    <row r="17" spans="4:4" x14ac:dyDescent="0.3">
-      <c r="D17" s="4"/>
-    </row>
-    <row r="18" spans="4:4" x14ac:dyDescent="0.3">
-      <c r="D18" s="4"/>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A17" s="1">
+        <v>4</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="D17" s="1">
+        <v>1.24</v>
+      </c>
+      <c r="E17" s="4">
+        <v>1.01</v>
+      </c>
+      <c r="F17" s="25">
+        <v>2.04</v>
+      </c>
+      <c r="G17" s="1">
+        <v>24</v>
+      </c>
+      <c r="H17" s="1">
+        <v>39.5</v>
+      </c>
+      <c r="I17" s="1">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A18" s="1">
+        <v>4</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="D18" s="1">
+        <v>1.01</v>
+      </c>
+      <c r="E18" s="39">
+        <v>0.71899999999999997</v>
+      </c>
+      <c r="F18" s="1">
+        <v>0.82399999999999995</v>
+      </c>
+      <c r="G18" s="1">
+        <v>20</v>
+      </c>
+      <c r="H18" s="1">
+        <v>43.1</v>
+      </c>
+      <c r="I18" s="1">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A19" s="1">
+        <v>4</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="D19" s="1">
+        <v>0.82399999999999995</v>
+      </c>
+      <c r="E19" s="39">
+        <v>0.44500000000000001</v>
+      </c>
+      <c r="F19" s="25">
+        <v>1.36</v>
+      </c>
+      <c r="G19" s="1">
+        <v>40</v>
+      </c>
+      <c r="H19" s="1">
+        <v>66.2</v>
+      </c>
+      <c r="I19" s="1">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A20" s="1">
+        <v>5</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="D20" s="1">
+        <v>1.04</v>
+      </c>
+      <c r="E20" s="25">
+        <v>0.91800000000000004</v>
+      </c>
+      <c r="F20" s="25">
+        <v>1.76</v>
+      </c>
+      <c r="G20" s="1">
+        <v>24</v>
+      </c>
+      <c r="H20" s="1">
+        <v>40.6</v>
+      </c>
+      <c r="I20" s="1">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A21" s="1">
+        <v>5</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="D21" s="1">
+        <v>0.91800000000000004</v>
+      </c>
+      <c r="E21" s="1">
+        <v>0.71499999999999997</v>
+      </c>
+      <c r="F21" s="1">
+        <v>0.79300000000000004</v>
+      </c>
+      <c r="G21" s="1">
+        <v>20</v>
+      </c>
+      <c r="H21" s="1">
+        <v>37.6</v>
+      </c>
+      <c r="I21" s="1">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A22" s="1">
+        <v>5</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="D22" s="1">
+        <v>0.79300000000000004</v>
+      </c>
+      <c r="E22" s="1">
+        <v>0.44700000000000001</v>
+      </c>
+      <c r="F22" s="25">
+        <v>1.27</v>
+      </c>
+      <c r="G22" s="1">
+        <v>40</v>
+      </c>
+      <c r="H22" s="1">
+        <v>63.8</v>
+      </c>
+      <c r="I22" s="1">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A23" s="1">
+        <v>4</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="D23" s="1">
+        <f>D17</f>
+        <v>1.24</v>
+      </c>
+      <c r="E23" s="39">
+        <f>AVERAGE(E18,E19)</f>
+        <v>0.58199999999999996</v>
+      </c>
+      <c r="F23" s="25">
+        <f>AVERAGE(F17,F19)</f>
+        <v>1.7000000000000002</v>
+      </c>
+      <c r="G23" s="1">
+        <v>30.080000000000002</v>
+      </c>
+      <c r="H23" s="1">
+        <v>56.761981000000006</v>
+      </c>
+      <c r="I23" s="1">
+        <v>152.5</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A24" s="1">
+        <v>5</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="D24" s="1">
+        <f>D20</f>
+        <v>1.04</v>
+      </c>
+      <c r="E24" s="39">
+        <f>AVERAGE(E21:E22)</f>
+        <v>0.58099999999999996</v>
+      </c>
+      <c r="F24" s="25">
+        <f>AVERAGE(F20,F22)</f>
+        <v>1.5150000000000001</v>
+      </c>
+      <c r="G24" s="1">
+        <v>30.080000000000002</v>
+      </c>
+      <c r="H24" s="1">
+        <v>54.849347199999997</v>
+      </c>
+      <c r="I24" s="1">
+        <v>116</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
@@ -4960,6 +6057,707 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4728730A-4531-47D1-BC67-8C18E3CB3687}">
+  <dimension ref="A1:AMK24"/>
+  <sheetViews>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D20" sqref="D20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="8.88671875" style="1"/>
+    <col min="2" max="3" width="10.33203125" style="1" customWidth="1"/>
+    <col min="4" max="18" width="8.88671875" style="1"/>
+    <col min="19" max="19" width="17.109375" style="1" customWidth="1"/>
+    <col min="20" max="1025" width="8.88671875" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A1" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="I1" s="21" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="2" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A2" s="1">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="D2" s="1">
+        <f>out!E2</f>
+        <v>1.38</v>
+      </c>
+      <c r="E2" s="1">
+        <f>out!E4</f>
+        <v>1.08</v>
+      </c>
+      <c r="F2" s="1">
+        <f>out!E3</f>
+        <v>2.2799999999999998</v>
+      </c>
+      <c r="G2" s="4">
+        <v>25.081389940867702</v>
+      </c>
+      <c r="H2" s="4">
+        <v>41.438818163172797</v>
+      </c>
+      <c r="I2" s="19">
+        <v>41</v>
+      </c>
+      <c r="S2" s="4"/>
+    </row>
+    <row r="3" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A3" s="1">
+        <v>2</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="D3" s="1">
+        <f>out!E9</f>
+        <v>1.62</v>
+      </c>
+      <c r="E3" s="1">
+        <f>out!E11</f>
+        <v>1.34</v>
+      </c>
+      <c r="F3" s="1">
+        <f>out!E10</f>
+        <v>2.61</v>
+      </c>
+      <c r="G3" s="4">
+        <v>25.025977140116701</v>
+      </c>
+      <c r="H3" s="4">
+        <v>40.319629836854702</v>
+      </c>
+      <c r="I3" s="19">
+        <v>91</v>
+      </c>
+      <c r="S3" s="4"/>
+    </row>
+    <row r="4" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A4" s="1">
+        <v>3</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="D4" s="1">
+        <f>out!E16</f>
+        <v>0.98</v>
+      </c>
+      <c r="E4" s="1">
+        <f>out!E18</f>
+        <v>0.8</v>
+      </c>
+      <c r="F4" s="1">
+        <f>out!E17</f>
+        <v>1.39</v>
+      </c>
+      <c r="G4" s="4">
+        <v>25.1222057450431</v>
+      </c>
+      <c r="H4" s="4">
+        <v>35.632516311846899</v>
+      </c>
+      <c r="I4" s="19">
+        <v>71</v>
+      </c>
+      <c r="S4" s="4"/>
+    </row>
+    <row r="5" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A5" s="1">
+        <v>1</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="D5" s="1">
+        <f>E2</f>
+        <v>1.08</v>
+      </c>
+      <c r="E5" s="1">
+        <f>out!E5</f>
+        <v>0.78</v>
+      </c>
+      <c r="F5" s="1">
+        <f>out!E6</f>
+        <v>0.91</v>
+      </c>
+      <c r="G5" s="4">
+        <v>22.027475130269998</v>
+      </c>
+      <c r="H5" s="4">
+        <v>43.686509816306099</v>
+      </c>
+      <c r="I5" s="19">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="6" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A6" s="1">
+        <v>2</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="D6" s="1">
+        <f>E3</f>
+        <v>1.34</v>
+      </c>
+      <c r="E6" s="1">
+        <f>out!E12</f>
+        <v>0.91</v>
+      </c>
+      <c r="F6" s="1">
+        <f>out!E13</f>
+        <v>1.1200000000000001</v>
+      </c>
+      <c r="G6" s="4">
+        <v>22.0036790717419</v>
+      </c>
+      <c r="H6" s="4">
+        <v>47.032349220362001</v>
+      </c>
+      <c r="I6" s="19">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="7" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A7" s="1">
+        <v>3</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="D7" s="1">
+        <f>E4</f>
+        <v>0.8</v>
+      </c>
+      <c r="E7" s="1">
+        <f>out!E19</f>
+        <v>0.6</v>
+      </c>
+      <c r="F7" s="1">
+        <f>out!E20</f>
+        <v>0.64</v>
+      </c>
+      <c r="G7" s="4">
+        <v>21.969909354266001</v>
+      </c>
+      <c r="H7" s="4">
+        <v>41.477432015699499</v>
+      </c>
+      <c r="I7" s="19">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="8" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A8" s="1">
+        <v>1</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="D8" s="1">
+        <f>F5</f>
+        <v>0.91</v>
+      </c>
+      <c r="E8" s="1">
+        <f>out!E7</f>
+        <v>0.46</v>
+      </c>
+      <c r="F8" s="1">
+        <f>out!E8</f>
+        <v>1.52</v>
+      </c>
+      <c r="G8" s="4">
+        <v>42.033898305084698</v>
+      </c>
+      <c r="H8" s="4">
+        <v>70.210467498603094</v>
+      </c>
+      <c r="I8" s="19">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="9" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A9" s="1">
+        <v>2</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="D9" s="1">
+        <f>F6</f>
+        <v>1.1200000000000001</v>
+      </c>
+      <c r="E9" s="1">
+        <f>out!E14</f>
+        <v>0.52</v>
+      </c>
+      <c r="F9" s="1">
+        <f>out!E15</f>
+        <v>1.93</v>
+      </c>
+      <c r="G9" s="4">
+        <v>41.833478387003197</v>
+      </c>
+      <c r="H9" s="4">
+        <v>72.088047577603703</v>
+      </c>
+      <c r="I9" s="19">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="10" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A10" s="1">
+        <v>3</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="D10" s="1">
+        <f>F7</f>
+        <v>0.64</v>
+      </c>
+      <c r="E10" s="1">
+        <f>out!E21</f>
+        <v>0.39</v>
+      </c>
+      <c r="F10" s="1">
+        <f>out!E22</f>
+        <v>0.98</v>
+      </c>
+      <c r="G10" s="4">
+        <v>38.324386503067501</v>
+      </c>
+      <c r="H10" s="4">
+        <v>58.684216832822102</v>
+      </c>
+      <c r="I10" s="19">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="11" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A11" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="D11" s="4">
+        <f>_xlfn.STDEV.P(D2:D4)</f>
+        <v>0.26398653164297781</v>
+      </c>
+      <c r="E11" s="4">
+        <f>_xlfn.STDEV.P(E2:E4)</f>
+        <v>0.22050447211388433</v>
+      </c>
+      <c r="F11" s="4">
+        <f>_xlfn.STDEV.P(F2:F4)</f>
+        <v>0.51525613910839441</v>
+      </c>
+      <c r="G11" s="4">
+        <f>_xlfn.STDEV.P(G2:G4)</f>
+        <v>3.943553496761161E-2</v>
+      </c>
+      <c r="H11" s="4">
+        <f>_xlfn.STDEV.P(H2:H4)</f>
+        <v>2.5151707893144999</v>
+      </c>
+      <c r="I11" s="19">
+        <v>18.19732762431795</v>
+      </c>
+    </row>
+    <row r="12" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A12" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="D12" s="4">
+        <f>_xlfn.STDEV.P(D5:D7)</f>
+        <v>0.22050447211388433</v>
+      </c>
+      <c r="E12" s="4">
+        <f>_xlfn.STDEV.P(E5:E7)</f>
+        <v>0.12710450643291726</v>
+      </c>
+      <c r="F12" s="4">
+        <f>_xlfn.STDEV.P(F5:F7)</f>
+        <v>0.19646882704388513</v>
+      </c>
+      <c r="G12" s="4">
+        <f>_xlfn.STDEV.P(G5:G7)</f>
+        <v>2.3618412748477768E-2</v>
+      </c>
+      <c r="H12" s="4">
+        <f>_xlfn.STDEV.P(H5:H7)</f>
+        <v>2.2835588987738102</v>
+      </c>
+      <c r="I12" s="19">
+        <v>-10.293878958713464</v>
+      </c>
+    </row>
+    <row r="13" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A13" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="D13" s="4">
+        <f>_xlfn.STDEV.P(D8:D10)</f>
+        <v>0.19646882704388513</v>
+      </c>
+      <c r="E13" s="4">
+        <f>_xlfn.STDEV.P(E8:E10)</f>
+        <v>5.3124591501697516E-2</v>
+      </c>
+      <c r="F13" s="4">
+        <f>_xlfn.STDEV.P(F8:F10)</f>
+        <v>0.38904441334577178</v>
+      </c>
+      <c r="G13" s="4">
+        <f>_xlfn.STDEV.P(G8:G10)</f>
+        <v>1.703407428354905</v>
+      </c>
+      <c r="H13" s="4">
+        <f>_xlfn.STDEV.P(H8:H10)</f>
+        <v>5.9258608375889077</v>
+      </c>
+      <c r="I13" s="19">
+        <v>18.907097433455025</v>
+      </c>
+    </row>
+    <row r="14" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A14" s="1">
+        <v>1</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="D14" s="1">
+        <f>D2</f>
+        <v>1.38</v>
+      </c>
+      <c r="E14" s="4">
+        <f>AVERAGE(E5,E8)</f>
+        <v>0.62</v>
+      </c>
+      <c r="F14" s="25">
+        <f>AVERAGE(F2,F8)</f>
+        <v>1.9</v>
+      </c>
+      <c r="H14" s="4">
+        <v>59.400998287645102</v>
+      </c>
+      <c r="I14" s="19">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="15" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A15" s="1">
+        <v>2</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="D15" s="1">
+        <f>D3</f>
+        <v>1.62</v>
+      </c>
+      <c r="E15" s="4">
+        <f t="shared" ref="E15:E16" si="0">AVERAGE(E6,E9)</f>
+        <v>0.71500000000000008</v>
+      </c>
+      <c r="F15" s="25">
+        <f t="shared" ref="F15:F16" si="1">AVERAGE(F3,F9)</f>
+        <v>2.27</v>
+      </c>
+      <c r="H15" s="4">
+        <v>60.554081661965597</v>
+      </c>
+      <c r="I15" s="19">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="16" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A16" s="1">
+        <v>3</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="D16" s="1">
+        <f>D4</f>
+        <v>0.98</v>
+      </c>
+      <c r="E16" s="4">
+        <f t="shared" si="0"/>
+        <v>0.495</v>
+      </c>
+      <c r="F16" s="25">
+        <f t="shared" si="1"/>
+        <v>1.1850000000000001</v>
+      </c>
+      <c r="H16" s="4">
+        <v>51.300016366594399</v>
+      </c>
+      <c r="I16" s="19">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A17" s="1">
+        <v>4</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="D17" s="1">
+        <v>1.24</v>
+      </c>
+      <c r="E17" s="4">
+        <v>1.01</v>
+      </c>
+      <c r="F17" s="25">
+        <v>2.04</v>
+      </c>
+      <c r="G17" s="1">
+        <v>24</v>
+      </c>
+      <c r="H17" s="1">
+        <v>39.5</v>
+      </c>
+      <c r="I17" s="1">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A18" s="1">
+        <v>4</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="D18" s="1">
+        <v>1.01</v>
+      </c>
+      <c r="E18" s="39">
+        <v>0.71899999999999997</v>
+      </c>
+      <c r="F18" s="1">
+        <v>0.82399999999999995</v>
+      </c>
+      <c r="G18" s="1">
+        <v>20</v>
+      </c>
+      <c r="H18" s="1">
+        <v>43.1</v>
+      </c>
+      <c r="I18" s="1">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A19" s="1">
+        <v>4</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="D19" s="1">
+        <v>0.82399999999999995</v>
+      </c>
+      <c r="E19" s="39">
+        <v>0.44500000000000001</v>
+      </c>
+      <c r="F19" s="25">
+        <v>1.36</v>
+      </c>
+      <c r="G19" s="1">
+        <v>40</v>
+      </c>
+      <c r="H19" s="1">
+        <v>66.2</v>
+      </c>
+      <c r="I19" s="1">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A20" s="1">
+        <v>5</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="D20" s="1">
+        <v>1.04</v>
+      </c>
+      <c r="E20" s="25">
+        <v>0.91800000000000004</v>
+      </c>
+      <c r="F20" s="25">
+        <v>1.76</v>
+      </c>
+      <c r="G20" s="1">
+        <v>24</v>
+      </c>
+      <c r="H20" s="1">
+        <v>40.6</v>
+      </c>
+      <c r="I20" s="1">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A21" s="1">
+        <v>5</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="D21" s="1">
+        <v>0.91800000000000004</v>
+      </c>
+      <c r="E21" s="1">
+        <v>0.71499999999999997</v>
+      </c>
+      <c r="F21" s="1">
+        <v>0.79300000000000004</v>
+      </c>
+      <c r="G21" s="1">
+        <v>20</v>
+      </c>
+      <c r="H21" s="1">
+        <v>37.6</v>
+      </c>
+      <c r="I21" s="1">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A22" s="1">
+        <v>5</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="D22" s="1">
+        <v>0.79300000000000004</v>
+      </c>
+      <c r="E22" s="1">
+        <v>0.44700000000000001</v>
+      </c>
+      <c r="F22" s="25">
+        <v>1.27</v>
+      </c>
+      <c r="G22" s="1">
+        <v>40</v>
+      </c>
+      <c r="H22" s="1">
+        <v>63.8</v>
+      </c>
+      <c r="I22" s="1">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A23" s="1">
+        <v>4</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="D23" s="1">
+        <f>D17</f>
+        <v>1.24</v>
+      </c>
+      <c r="E23" s="39">
+        <f>AVERAGE(E18,E19)</f>
+        <v>0.58199999999999996</v>
+      </c>
+      <c r="F23" s="25">
+        <f>AVERAGE(F17,F19)</f>
+        <v>1.7000000000000002</v>
+      </c>
+      <c r="G23" s="1">
+        <v>30.080000000000002</v>
+      </c>
+      <c r="H23" s="1">
+        <v>56.761981000000006</v>
+      </c>
+      <c r="I23" s="1">
+        <v>152.5</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A24" s="1">
+        <v>5</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="D24" s="1">
+        <f>D20</f>
+        <v>1.04</v>
+      </c>
+      <c r="E24" s="39">
+        <f>AVERAGE(E21:E22)</f>
+        <v>0.58099999999999996</v>
+      </c>
+      <c r="F24" s="25">
+        <f>AVERAGE(F20,F22)</f>
+        <v>1.5150000000000001</v>
+      </c>
+      <c r="G24" s="1">
+        <v>30.080000000000002</v>
+      </c>
+      <c r="H24" s="1">
+        <v>54.849347199999997</v>
+      </c>
+      <c r="I24" s="1">
+        <v>116</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{69F48122-4A28-482A-9135-507475642A28}">
   <dimension ref="A1"/>
   <sheetViews>

</xml_diff>